<commit_message>
Updated budget allocation rescaling after optimization to prevent over spending
</commit_message>
<xml_diff>
--- a/tests/optim_results.xlsx
+++ b/tests/optim_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="40">
   <si>
     <t>Scenario</t>
   </si>
@@ -80,7 +80,7 @@
     <t>test2 (x1)</t>
   </si>
   <si>
-    <t>test2 (x2)</t>
+    <t>test2 (x10)</t>
   </si>
   <si>
     <t>Program</t>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Budget</t>
+  </si>
+  <si>
+    <t>Excess budget</t>
   </si>
 </sst>
 </file>
@@ -1341,46 +1344,46 @@
         <v>0</v>
       </c>
       <c r="D18" s="3">
-        <v>1197004.541552285</v>
+        <v>1181989.216507733</v>
       </c>
       <c r="E18" s="3">
-        <v>1207291.772076862</v>
+        <v>1199295.611394636</v>
       </c>
       <c r="F18" s="3">
-        <v>1216623.788480173</v>
+        <v>1214453.471733304</v>
       </c>
       <c r="G18" s="3">
-        <v>1226223.210974244</v>
+        <v>1228534.148725318</v>
       </c>
       <c r="H18" s="3">
-        <v>1238182.526159477</v>
+        <v>1243849.139552845</v>
       </c>
       <c r="I18" s="3">
-        <v>1253064.26796553</v>
+        <v>1261229.186969528</v>
       </c>
       <c r="J18" s="3">
-        <v>1270996.752944946</v>
+        <v>1281035.805201516</v>
       </c>
       <c r="K18" s="3">
-        <v>1291357.090552277</v>
+        <v>1302819.912009235</v>
       </c>
       <c r="L18" s="3">
-        <v>1313614.072062191</v>
+        <v>1326178.817375609</v>
       </c>
       <c r="M18" s="3">
-        <v>1337856.345200946</v>
+        <v>1351300.169581505</v>
       </c>
       <c r="N18" s="3">
-        <v>1363556.286737453</v>
+        <v>1377720.500885826</v>
       </c>
       <c r="O18" s="3">
-        <v>1390183.457752442</v>
+        <v>1404953.535417152</v>
       </c>
       <c r="P18" s="3">
-        <v>1417692.374871914</v>
+        <v>1432989.292167476</v>
       </c>
       <c r="Q18" s="3">
-        <v>16723646.48733074</v>
+        <v>16806348.80752169</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1392,46 +1395,46 @@
         <v>0</v>
       </c>
       <c r="D19" s="3">
-        <v>190340.2151039458</v>
+        <v>192227.6281062525</v>
       </c>
       <c r="E19" s="3">
-        <v>192786.418087082</v>
+        <v>194512.2049523072</v>
       </c>
       <c r="F19" s="3">
-        <v>195600.3648859152</v>
+        <v>197214.5120773835</v>
       </c>
       <c r="G19" s="3">
-        <v>198598.6510826958</v>
+        <v>200140.6906862723</v>
       </c>
       <c r="H19" s="3">
-        <v>202269.4199823656</v>
+        <v>203765.9364240069</v>
       </c>
       <c r="I19" s="3">
-        <v>206201.5113888693</v>
+        <v>207673.4835987023</v>
       </c>
       <c r="J19" s="3">
-        <v>209747.3607432851</v>
+        <v>211212.0562242885</v>
       </c>
       <c r="K19" s="3">
-        <v>214292.4916873257</v>
+        <v>215758.275910671</v>
       </c>
       <c r="L19" s="3">
-        <v>218627.1097363443</v>
+        <v>220103.5072589556</v>
       </c>
       <c r="M19" s="3">
-        <v>222939.4117639836</v>
+        <v>224433.3859193905</v>
       </c>
       <c r="N19" s="3">
-        <v>227280.4485122933</v>
+        <v>228796.1954772036</v>
       </c>
       <c r="O19" s="3">
-        <v>232170.9323198436</v>
+        <v>233710.1750829767</v>
       </c>
       <c r="P19" s="3">
-        <v>236703.6055629714</v>
+        <v>238270.3899960906</v>
       </c>
       <c r="Q19" s="3">
-        <v>2747557.940856921</v>
+        <v>2767818.441714501</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1443,46 +1446,46 @@
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>740049.3764342512</v>
+        <v>754750.9718882912</v>
       </c>
       <c r="E20" s="3">
-        <v>739302.6990187386</v>
+        <v>746519.9289767036</v>
       </c>
       <c r="F20" s="3">
-        <v>740288.1146367028</v>
+        <v>741389.9114838012</v>
       </c>
       <c r="G20" s="3">
-        <v>743041.9106352483</v>
+        <v>739499.5810406806</v>
       </c>
       <c r="H20" s="3">
-        <v>748206.235452348</v>
+        <v>741218.1271043523</v>
       </c>
       <c r="I20" s="3">
-        <v>755756.8348545531</v>
+        <v>746219.6238528547</v>
       </c>
       <c r="J20" s="3">
-        <v>765558.6506955943</v>
+        <v>754116.9500983079</v>
       </c>
       <c r="K20" s="3">
-        <v>777105.347510229</v>
+        <v>764219.3483201743</v>
       </c>
       <c r="L20" s="3">
-        <v>789990.7810276311</v>
+        <v>775986.3100367729</v>
       </c>
       <c r="M20" s="3">
-        <v>804208.752734701</v>
+        <v>789309.3616371341</v>
       </c>
       <c r="N20" s="3">
-        <v>819401.1202115066</v>
+        <v>803764.4032511218</v>
       </c>
       <c r="O20" s="3">
-        <v>835220.3631253733</v>
+        <v>818958.9810379207</v>
       </c>
       <c r="P20" s="3">
-        <v>851618.7173685551</v>
+        <v>834809.6220345102</v>
       </c>
       <c r="Q20" s="3">
-        <v>10109748.90370543</v>
+        <v>10010763.12076263</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1494,46 +1497,46 @@
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>55104.83230441622</v>
+        <v>57261.66778613837</v>
       </c>
       <c r="E21" s="3">
-        <v>55376.23960716846</v>
+        <v>57529.98967720375</v>
       </c>
       <c r="F21" s="3">
-        <v>55669.74736968627</v>
+        <v>57826.47291697245</v>
       </c>
       <c r="G21" s="3">
-        <v>56021.16868384515</v>
+        <v>58186.89274946359</v>
       </c>
       <c r="H21" s="3">
-        <v>56508.29777302948</v>
+        <v>58690.50636606054</v>
       </c>
       <c r="I21" s="3">
-        <v>57146.44748533145</v>
+        <v>59352.23918608791</v>
       </c>
       <c r="J21" s="3">
-        <v>57935.42603755477</v>
+        <v>60171.33411401763</v>
       </c>
       <c r="K21" s="3">
-        <v>58843.10948654273</v>
+        <v>61114.09064316124</v>
       </c>
       <c r="L21" s="3">
-        <v>59842.83224535232</v>
+        <v>62152.6221631123</v>
       </c>
       <c r="M21" s="3">
-        <v>60936.93980887278</v>
+        <v>63289.26955246255</v>
       </c>
       <c r="N21" s="3">
-        <v>62100.23413423735</v>
+        <v>64497.79098383798</v>
       </c>
       <c r="O21" s="3">
-        <v>63307.73925309573</v>
+        <v>65752.20593122006</v>
       </c>
       <c r="P21" s="3">
-        <v>64556.80248407614</v>
+        <v>67049.75133414545</v>
       </c>
       <c r="Q21" s="3">
-        <v>763349.8166732088</v>
+        <v>792874.8334038837</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1545,46 +1548,46 @@
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>406081.6644992621</v>
+        <v>406015.8946034763</v>
       </c>
       <c r="E22" s="3">
-        <v>408081.7346319509</v>
+        <v>407918.4405273829</v>
       </c>
       <c r="F22" s="3">
-        <v>410244.6687297856</v>
+        <v>410020.6654971341</v>
       </c>
       <c r="G22" s="3">
-        <v>412834.3826664111</v>
+        <v>412576.235154453</v>
       </c>
       <c r="H22" s="3">
-        <v>416424.1620576121</v>
+        <v>416147.1254372994</v>
       </c>
       <c r="I22" s="3">
-        <v>421126.8512145219</v>
+        <v>420839.1655629091</v>
       </c>
       <c r="J22" s="3">
-        <v>426941.0368375019</v>
+        <v>426646.9873184792</v>
       </c>
       <c r="K22" s="3">
-        <v>433629.9893374795</v>
+        <v>433331.6360612139</v>
       </c>
       <c r="L22" s="3">
-        <v>440997.2031544545</v>
+        <v>440695.3807869467</v>
       </c>
       <c r="M22" s="3">
-        <v>449059.9628427735</v>
+        <v>448754.8195786941</v>
       </c>
       <c r="N22" s="3">
-        <v>457632.5775517149</v>
+        <v>457323.8838249531</v>
       </c>
       <c r="O22" s="3">
-        <v>466530.9929547157</v>
+        <v>466218.357680788</v>
       </c>
       <c r="P22" s="3">
-        <v>475735.6607613302</v>
+        <v>475418.6495675868</v>
       </c>
       <c r="Q22" s="3">
-        <v>5625320.887239514</v>
+        <v>5621907.241601316</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1596,43 +1599,43 @@
         <v>0.3411657413950535</v>
       </c>
       <c r="D23" s="3">
-        <v>0.3332178537377351</v>
+        <v>0.3319713853578362</v>
       </c>
       <c r="E23" s="3">
-        <v>0.3321008973055083</v>
+        <v>0.3285019485237618</v>
       </c>
       <c r="F23" s="3">
-        <v>0.3311046540908239</v>
+        <v>0.3258082683081363</v>
       </c>
       <c r="G23" s="3">
-        <v>0.3303792407229778</v>
+        <v>0.3238696551527901</v>
       </c>
       <c r="H23" s="3">
-        <v>0.3297580797476226</v>
+        <v>0.322389995205874</v>
       </c>
       <c r="I23" s="3">
-        <v>0.3293042058393114</v>
+        <v>0.3213292496712262</v>
       </c>
       <c r="J23" s="3">
-        <v>0.3291043324384335</v>
+        <v>0.3207016870713299</v>
       </c>
       <c r="K23" s="3">
-        <v>0.3287879904235446</v>
+        <v>0.3200918879032547</v>
       </c>
       <c r="L23" s="3">
-        <v>0.3286391493558266</v>
+        <v>0.319733380517895</v>
       </c>
       <c r="M23" s="3">
-        <v>0.3285675229345156</v>
+        <v>0.3195161392807908</v>
       </c>
       <c r="N23" s="3">
-        <v>0.3285349729207786</v>
+        <v>0.3193830631449449</v>
       </c>
       <c r="O23" s="3">
-        <v>0.328427046286727</v>
+        <v>0.3192075236491017</v>
       </c>
       <c r="P23" s="3">
-        <v>0.3284395005251026</v>
+        <v>0.3191693840596564</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>10</v>
@@ -1647,43 +1650,43 @@
         <v>0.04535037632743646</v>
       </c>
       <c r="D24" s="3">
-        <v>0.04390779267785808</v>
+        <v>0.04500834598179335</v>
       </c>
       <c r="E24" s="3">
-        <v>0.0439718963831596</v>
+        <v>0.04507232859671784</v>
       </c>
       <c r="F24" s="3">
-        <v>0.04407312401367735</v>
+        <v>0.04517360941141138</v>
       </c>
       <c r="G24" s="3">
-        <v>0.04416311176512802</v>
+        <v>0.04526371927860786</v>
       </c>
       <c r="H24" s="3">
-        <v>0.04425981335951566</v>
+        <v>0.04536012612486847</v>
       </c>
       <c r="I24" s="3">
-        <v>0.04433723431138782</v>
+        <v>0.0454373888779136</v>
       </c>
       <c r="J24" s="3">
-        <v>0.04436381592118323</v>
+        <v>0.04546426024482765</v>
       </c>
       <c r="K24" s="3">
-        <v>0.0444246747167359</v>
+        <v>0.04552454249857287</v>
       </c>
       <c r="L24" s="3">
-        <v>0.04445289251032009</v>
+        <v>0.04555280305057728</v>
       </c>
       <c r="M24" s="3">
-        <v>0.04446405857430339</v>
+        <v>0.04556401862645677</v>
       </c>
       <c r="N24" s="3">
-        <v>0.04446606843639848</v>
+        <v>0.04556605934333807</v>
       </c>
       <c r="O24" s="3">
-        <v>0.0444882182387574</v>
+        <v>0.04558790309025865</v>
       </c>
       <c r="P24" s="3">
-        <v>0.04448350453487895</v>
+        <v>0.04558337933275754</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>10</v>
@@ -1698,43 +1701,43 @@
         <v>0.2195512735036556</v>
       </c>
       <c r="D25" s="3">
-        <v>0.2272103592637744</v>
+        <v>0.2272073429515667</v>
       </c>
       <c r="E25" s="3">
-        <v>0.2268542954355987</v>
+        <v>0.2268542352049324</v>
       </c>
       <c r="F25" s="3">
-        <v>0.2268081450134957</v>
+        <v>0.226809864282355</v>
       </c>
       <c r="G25" s="3">
-        <v>0.2268560468246319</v>
+        <v>0.2268586183348504</v>
       </c>
       <c r="H25" s="3">
-        <v>0.2268841438429211</v>
+        <v>0.2268870686948646</v>
       </c>
       <c r="I25" s="3">
-        <v>0.2269423180895502</v>
+        <v>0.2269453753700729</v>
       </c>
       <c r="J25" s="3">
-        <v>0.227032004003884</v>
+        <v>0.227035111363887</v>
       </c>
       <c r="K25" s="3">
-        <v>0.2270070097537967</v>
+        <v>0.2270100610609329</v>
       </c>
       <c r="L25" s="3">
-        <v>0.2270637783140593</v>
+        <v>0.2270667920616541</v>
       </c>
       <c r="M25" s="3">
-        <v>0.2270970136186378</v>
+        <v>0.2270999830369947</v>
       </c>
       <c r="N25" s="3">
-        <v>0.2271134890073924</v>
+        <v>0.2271164152963361</v>
       </c>
       <c r="O25" s="3">
-        <v>0.2270915877607423</v>
+        <v>0.2270944562298374</v>
       </c>
       <c r="P25" s="3">
-        <v>0.2271289094524802</v>
+        <v>0.2271317571742888</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>10</v>
@@ -1749,46 +1752,46 @@
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>8115.764723595252</v>
+        <v>8115.766821694776</v>
       </c>
       <c r="E26" s="3">
-        <v>8269.61808328426</v>
+        <v>8269.620221158184</v>
       </c>
       <c r="F26" s="3">
-        <v>8461.934782895525</v>
+        <v>8461.936970487444</v>
       </c>
       <c r="G26" s="3">
-        <v>8615.788142584533</v>
+        <v>8615.79036995085</v>
       </c>
       <c r="H26" s="3">
-        <v>8769.641502273542</v>
+        <v>8769.643769414261</v>
       </c>
       <c r="I26" s="3">
-        <v>8961.958201884803</v>
+        <v>8961.960518743519</v>
       </c>
       <c r="J26" s="3">
-        <v>9154.274901496065</v>
+        <v>9154.277268072779</v>
       </c>
       <c r="K26" s="3">
-        <v>9308.128261185075</v>
+        <v>9308.130667536187</v>
       </c>
       <c r="L26" s="3">
-        <v>9538.908300718591</v>
+        <v>9538.910766731298</v>
       </c>
       <c r="M26" s="3">
-        <v>9731.225000329849</v>
+        <v>9731.227516060559</v>
       </c>
       <c r="N26" s="3">
-        <v>9923.541699941114</v>
+        <v>9923.544265389817</v>
       </c>
       <c r="O26" s="3">
-        <v>10115.85839955238</v>
+        <v>10115.86101471908</v>
       </c>
       <c r="P26" s="3">
-        <v>10346.63843908589</v>
+        <v>10346.64111391419</v>
       </c>
       <c r="Q26" s="3">
-        <v>119313.2804388269</v>
+        <v>119313.3112838729</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1800,46 +1803,46 @@
         <v>0</v>
       </c>
       <c r="D27" s="3">
-        <v>619519.225327066</v>
+        <v>619519.9932467644</v>
       </c>
       <c r="E27" s="3">
-        <v>633926.6491718815</v>
+        <v>633927.4349501774</v>
       </c>
       <c r="F27" s="3">
-        <v>645452.5882477339</v>
+        <v>645453.388312908</v>
       </c>
       <c r="G27" s="3">
-        <v>656978.5273235863</v>
+        <v>656979.3416756385</v>
       </c>
       <c r="H27" s="3">
-        <v>671385.9511684016</v>
+        <v>671386.7833790516</v>
       </c>
       <c r="I27" s="3">
-        <v>685793.3750132171</v>
+        <v>685794.2250824647</v>
       </c>
       <c r="J27" s="3">
-        <v>697319.3140890695</v>
+        <v>697320.1784451953</v>
       </c>
       <c r="K27" s="3">
-        <v>714608.2227028483</v>
+        <v>714609.1084892909</v>
       </c>
       <c r="L27" s="3">
-        <v>729015.6465476637</v>
+        <v>729016.5501927041</v>
       </c>
       <c r="M27" s="3">
-        <v>743423.0703924793</v>
+        <v>743423.9918961172</v>
       </c>
       <c r="N27" s="3">
-        <v>757830.4942372949</v>
+        <v>757831.4335995305</v>
       </c>
       <c r="O27" s="3">
-        <v>775119.4028510734</v>
+        <v>775120.3636436262</v>
       </c>
       <c r="P27" s="3">
-        <v>789526.8266958888</v>
+        <v>789527.8053470392</v>
       </c>
       <c r="Q27" s="3">
-        <v>9119899.293768205</v>
+        <v>9119910.598260507</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1851,43 +1854,43 @@
         <v>0.18698022</v>
       </c>
       <c r="D28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="E28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.245074041161066</v>
       </c>
       <c r="F28" s="3">
-        <v>0.2450737373820343</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="G28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.245074041161066</v>
       </c>
       <c r="H28" s="3">
-        <v>0.2450737373820341</v>
+        <v>0.245074041161066</v>
       </c>
       <c r="I28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="J28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="K28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="L28" s="3">
-        <v>0.2450737373820343</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="M28" s="3">
-        <v>0.2450737373820343</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="N28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.245074041161066</v>
       </c>
       <c r="O28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="P28" s="3">
-        <v>0.2450737373820342</v>
+        <v>0.2450740411610661</v>
       </c>
       <c r="Q28" s="3" t="s">
         <v>10</v>
@@ -2004,43 +2007,43 @@
         <v>0</v>
       </c>
       <c r="D31" s="3">
-        <v>88.53033260648643</v>
+        <v>89.40819911918722</v>
       </c>
       <c r="E31" s="3">
-        <v>88.07508808989145</v>
+        <v>88.90570874909417</v>
       </c>
       <c r="F31" s="3">
-        <v>87.81896784172125</v>
+        <v>88.61219197814009</v>
       </c>
       <c r="G31" s="3">
-        <v>87.63536067188711</v>
+        <v>88.39853842415056</v>
       </c>
       <c r="H31" s="3">
-        <v>87.46384545910753</v>
+        <v>88.20187252198414</v>
       </c>
       <c r="I31" s="3">
-        <v>87.31933582701575</v>
+        <v>88.03641059240977</v>
       </c>
       <c r="J31" s="3">
-        <v>87.22149632963492</v>
+        <v>87.92165700432582</v>
       </c>
       <c r="K31" s="3">
-        <v>87.11236109098942</v>
+        <v>87.79787813743962</v>
       </c>
       <c r="L31" s="3">
-        <v>87.02825048537976</v>
+        <v>87.70148954016372</v>
       </c>
       <c r="M31" s="3">
-        <v>86.9607017576012</v>
+        <v>87.62364057474481</v>
       </c>
       <c r="N31" s="3">
-        <v>86.9063082751375</v>
+        <v>87.56055974963515</v>
       </c>
       <c r="O31" s="3">
-        <v>86.85072069505185</v>
+        <v>87.49733835068869</v>
       </c>
       <c r="P31" s="3">
-        <v>86.81067743623763</v>
+        <v>87.45081964342813</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>10</v>
@@ -2055,43 +2058,43 @@
         <v>0</v>
       </c>
       <c r="D32" s="3">
-        <v>3.774774290044303</v>
+        <v>3.774775265904547</v>
       </c>
       <c r="E32" s="3">
-        <v>3.766754668248164</v>
+        <v>3.766755642035163</v>
       </c>
       <c r="F32" s="3">
-        <v>3.770457904366471</v>
+        <v>3.770458879110835</v>
       </c>
       <c r="G32" s="3">
-        <v>3.772616204324642</v>
+        <v>3.772617179626973</v>
       </c>
       <c r="H32" s="3">
-        <v>3.770781003092243</v>
+        <v>3.770781977920135</v>
       </c>
       <c r="I32" s="3">
-        <v>3.769860488697932</v>
+        <v>3.769861463287852</v>
       </c>
       <c r="J32" s="3">
-        <v>3.771811271125874</v>
+        <v>3.771812246220114</v>
       </c>
       <c r="K32" s="3">
-        <v>3.769324058398217</v>
+        <v>3.769325032849459</v>
       </c>
       <c r="L32" s="3">
-        <v>3.769443926697651</v>
+        <v>3.769444901179881</v>
       </c>
       <c r="M32" s="3">
-        <v>3.769700801197436</v>
+        <v>3.769701775746073</v>
       </c>
       <c r="N32" s="3">
-        <v>3.770052768885912</v>
+        <v>3.770053743525541</v>
       </c>
       <c r="O32" s="3">
-        <v>3.769167831191318</v>
+        <v>3.769168805602171</v>
       </c>
       <c r="P32" s="3">
-        <v>3.769771893801797</v>
+        <v>3.769772868368814</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>10</v>
@@ -2124,46 +2127,46 @@
         <v>0</v>
       </c>
       <c r="D34" s="3">
-        <v>1205442.181495192</v>
+        <v>1207232.89238433</v>
       </c>
       <c r="E34" s="3">
-        <v>1227677.360018433</v>
+        <v>1233725.781504772</v>
       </c>
       <c r="F34" s="3">
-        <v>1246848.799900643</v>
+        <v>1257245.393933501</v>
       </c>
       <c r="G34" s="3">
-        <v>1264077.95805579</v>
+        <v>1278298.590862266</v>
       </c>
       <c r="H34" s="3">
-        <v>1281880.950140108</v>
+        <v>1299195.133325367</v>
       </c>
       <c r="I34" s="3">
-        <v>1301275.845737921</v>
+        <v>1321017.758795508</v>
       </c>
       <c r="J34" s="3">
-        <v>1322777.909823682</v>
+        <v>1344429.304415835</v>
       </c>
       <c r="K34" s="3">
-        <v>1346034.366973016</v>
+        <v>1369208.95822366</v>
       </c>
       <c r="L34" s="3">
-        <v>1370711.367597485</v>
+        <v>1395129.734500986</v>
       </c>
       <c r="M34" s="3">
-        <v>1397062.474442236</v>
+        <v>1422535.739857886</v>
       </c>
       <c r="N34" s="3">
-        <v>1424651.869428715</v>
+        <v>1451045.753453505</v>
       </c>
       <c r="O34" s="3">
-        <v>1453007.525826905</v>
+        <v>1480224.06905238</v>
       </c>
       <c r="P34" s="3">
-        <v>1482140.524296434</v>
+        <v>1510114.350366139</v>
       </c>
       <c r="Q34" s="3">
-        <v>17323589.13373656</v>
+        <v>17569403.46067613</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2175,46 +2178,46 @@
         <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>188327.8120740966</v>
+        <v>187936.8823004595</v>
       </c>
       <c r="E35" s="3">
-        <v>190563.2923147606</v>
+        <v>189956.1252965385</v>
       </c>
       <c r="F35" s="3">
-        <v>193210.1030009195</v>
+        <v>192498.3971518383</v>
       </c>
       <c r="G35" s="3">
-        <v>196077.0004000688</v>
+        <v>195295.4943641174</v>
       </c>
       <c r="H35" s="3">
-        <v>199638.3239461579</v>
+        <v>198803.196570622</v>
       </c>
       <c r="I35" s="3">
-        <v>203474.3075235731</v>
+        <v>202595.1246588673</v>
       </c>
       <c r="J35" s="3">
-        <v>206936.5061237104</v>
+        <v>206020.7994625776</v>
       </c>
       <c r="K35" s="3">
-        <v>211403.83045668</v>
+        <v>210456.4985790247</v>
       </c>
       <c r="L35" s="3">
-        <v>215662.646010144</v>
+        <v>214685.8034842508</v>
       </c>
       <c r="M35" s="3">
-        <v>219903.7455897326</v>
+        <v>218900.1650728914</v>
       </c>
       <c r="N35" s="3">
-        <v>224176.3007219375</v>
+        <v>223147.8227001711</v>
       </c>
       <c r="O35" s="3">
-        <v>228997.6965020237</v>
+        <v>227944.8981198425</v>
       </c>
       <c r="P35" s="3">
-        <v>233461.3536086352</v>
+        <v>232384.4184709669</v>
       </c>
       <c r="Q35" s="3">
-        <v>2711832.91827244</v>
+        <v>2700625.626232169</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2226,46 +2229,46 @@
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>731696.6403388246</v>
+        <v>729915.4085144119</v>
       </c>
       <c r="E36" s="3">
-        <v>719299.3281115828</v>
+        <v>713320.9954999769</v>
       </c>
       <c r="F36" s="3">
-        <v>710861.9892181027</v>
+        <v>700648.0964036074</v>
       </c>
       <c r="G36" s="3">
-        <v>706402.0834548755</v>
+        <v>692497.2052313259</v>
       </c>
       <c r="H36" s="3">
-        <v>706083.8837497209</v>
+        <v>689212.8430939509</v>
       </c>
       <c r="I36" s="3">
-        <v>709418.3352059232</v>
+        <v>690230.3905161001</v>
       </c>
       <c r="J36" s="3">
-        <v>715891.3168766542</v>
+        <v>694886.6295932599</v>
       </c>
       <c r="K36" s="3">
-        <v>724737.7305978396</v>
+        <v>702286.5250977926</v>
       </c>
       <c r="L36" s="3">
-        <v>735364.2820586931</v>
+        <v>711732.7402173075</v>
       </c>
       <c r="M36" s="3">
-        <v>747608.9815887529</v>
+        <v>722975.72564181</v>
       </c>
       <c r="N36" s="3">
-        <v>761028.6991843445</v>
+        <v>735520.1853703291</v>
       </c>
       <c r="O36" s="3">
-        <v>775222.2474439046</v>
+        <v>748930.419567914</v>
       </c>
       <c r="P36" s="3">
-        <v>790089.0361353776</v>
+        <v>763074.7333147051</v>
       </c>
       <c r="Q36" s="3">
-        <v>9533704.553964596</v>
+        <v>9295231.89806249</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2277,46 +2280,46 @@
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>54795.25120929174</v>
+        <v>54795.51934068582</v>
       </c>
       <c r="E37" s="3">
-        <v>55073.5319132747</v>
+        <v>55075.51449575907</v>
       </c>
       <c r="F37" s="3">
-        <v>55377.16413289355</v>
+        <v>55382.33214617357</v>
       </c>
       <c r="G37" s="3">
-        <v>55738.36405552363</v>
+        <v>55747.29570848362</v>
       </c>
       <c r="H37" s="3">
-        <v>56232.95101024248</v>
+        <v>56245.48604694257</v>
       </c>
       <c r="I37" s="3">
-        <v>56875.88907312677</v>
+        <v>56891.55900629392</v>
       </c>
       <c r="J37" s="3">
-        <v>57667.21060493476</v>
+        <v>57685.50381605773</v>
       </c>
       <c r="K37" s="3">
-        <v>58575.29465862385</v>
+        <v>58595.75684929314</v>
       </c>
       <c r="L37" s="3">
-        <v>59573.91539932229</v>
+        <v>59596.17207832248</v>
       </c>
       <c r="M37" s="3">
-        <v>60665.66312648347</v>
+        <v>60689.42421646688</v>
       </c>
       <c r="N37" s="3">
-        <v>61825.67530551624</v>
+        <v>61850.71950088612</v>
       </c>
       <c r="O37" s="3">
-        <v>63029.25159633139</v>
+        <v>63055.40873556218</v>
       </c>
       <c r="P37" s="3">
-        <v>64273.86006913038</v>
+        <v>64301.00180873069</v>
       </c>
       <c r="Q37" s="3">
-        <v>759704.0221546952</v>
+        <v>759911.6937496578</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -2328,46 +2331,46 @@
         <v>0</v>
       </c>
       <c r="D38" s="3">
-        <v>406099.4636402088</v>
+        <v>406101.4508199901</v>
       </c>
       <c r="E38" s="3">
-        <v>408161.8621534897</v>
+        <v>408176.5555012845</v>
       </c>
       <c r="F38" s="3">
-        <v>410412.1462348627</v>
+        <v>410450.4474995669</v>
       </c>
       <c r="G38" s="3">
-        <v>413089.0770200999</v>
+        <v>413155.2714328714</v>
       </c>
       <c r="H38" s="3">
-        <v>416754.5679632405</v>
+        <v>416847.4678326319</v>
       </c>
       <c r="I38" s="3">
-        <v>421519.5210701059</v>
+        <v>421635.6543355625</v>
       </c>
       <c r="J38" s="3">
-        <v>427384.1761732779</v>
+        <v>427519.7511193061</v>
       </c>
       <c r="K38" s="3">
-        <v>434114.1835918923</v>
+        <v>434265.8333146751</v>
       </c>
       <c r="L38" s="3">
-        <v>441515.1779888092</v>
+        <v>441680.1270529146</v>
       </c>
       <c r="M38" s="3">
-        <v>449606.3566337825</v>
+        <v>449782.455213218</v>
       </c>
       <c r="N38" s="3">
-        <v>458203.4579030515</v>
+        <v>458389.0658541524</v>
       </c>
       <c r="O38" s="3">
-        <v>467123.422231406</v>
+        <v>467317.2784502856</v>
       </c>
       <c r="P38" s="3">
-        <v>476347.4849392346</v>
+        <v>476548.6382445064</v>
       </c>
       <c r="Q38" s="3">
-        <v>5630330.897543461</v>
+        <v>5631869.996670965</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -2379,43 +2382,43 @@
         <v>0.3411657413950535</v>
       </c>
       <c r="D39" s="3">
-        <v>0.3213473679273423</v>
+        <v>0.3160922745145809</v>
       </c>
       <c r="E39" s="3">
-        <v>0.3165646291682179</v>
+        <v>0.3091447504336624</v>
       </c>
       <c r="F39" s="3">
-        <v>0.3129606925841187</v>
+        <v>0.3040247943990836</v>
       </c>
       <c r="G39" s="3">
-        <v>0.3103837531296982</v>
+        <v>0.3003683350575914</v>
       </c>
       <c r="H39" s="3">
-        <v>0.3084637010826461</v>
+        <v>0.2976823746611954</v>
       </c>
       <c r="I39" s="3">
-        <v>0.3070966235966142</v>
+        <v>0.2957749598871964</v>
       </c>
       <c r="J39" s="3">
-        <v>0.3062459310508116</v>
+        <v>0.2945453429856479</v>
       </c>
       <c r="K39" s="3">
-        <v>0.3054929327313891</v>
+        <v>0.2935280423792215</v>
       </c>
       <c r="L39" s="3">
-        <v>0.3050305471390702</v>
+        <v>0.2928803353354885</v>
       </c>
       <c r="M39" s="3">
-        <v>0.3047378997752791</v>
+        <v>0.2924586433021583</v>
       </c>
       <c r="N39" s="3">
-        <v>0.3045503151429809</v>
+        <v>0.2921814131874236</v>
       </c>
       <c r="O39" s="3">
-        <v>0.3043434312891825</v>
+        <v>0.2919126266606309</v>
       </c>
       <c r="P39" s="3">
-        <v>0.3042772890235263</v>
+        <v>0.291802715422996</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>10</v>
@@ -2430,43 +2433,43 @@
         <v>0.04535037632743646</v>
       </c>
       <c r="D40" s="3">
-        <v>0.04362787627407355</v>
+        <v>0.04309255930226956</v>
       </c>
       <c r="E40" s="3">
-        <v>0.04369114105987361</v>
+        <v>0.04315490083743631</v>
       </c>
       <c r="F40" s="3">
-        <v>0.04379034646681258</v>
+        <v>0.04325098505820504</v>
       </c>
       <c r="G40" s="3">
-        <v>0.04387813596675981</v>
+        <v>0.04333544178168493</v>
       </c>
       <c r="H40" s="3">
-        <v>0.04397290466816944</v>
+        <v>0.04342675537479384</v>
       </c>
       <c r="I40" s="3">
-        <v>0.04404872681427938</v>
+        <v>0.04349966974085105</v>
       </c>
       <c r="J40" s="3">
-        <v>0.04407413975692315</v>
+        <v>0.04352364469695243</v>
       </c>
       <c r="K40" s="3">
-        <v>0.0441341256042669</v>
+        <v>0.04358165019530206</v>
       </c>
       <c r="L40" s="3">
-        <v>0.04416163817144216</v>
+        <v>0.04360795044569441</v>
       </c>
       <c r="M40" s="3">
-        <v>0.04417233390918089</v>
+        <v>0.04361804436626655</v>
       </c>
       <c r="N40" s="3">
-        <v>0.04417404981739383</v>
+        <v>0.04361953505699136</v>
       </c>
       <c r="O40" s="3">
-        <v>0.04419596417876492</v>
+        <v>0.04364079432591798</v>
       </c>
       <c r="P40" s="3">
-        <v>0.04419107161820696</v>
+        <v>0.04363586234625793</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>10</v>
@@ -2481,43 +2484,43 @@
         <v>0.2195512735036556</v>
       </c>
       <c r="D41" s="3">
-        <v>0.2270204521397145</v>
+        <v>0.2189713419349589</v>
       </c>
       <c r="E41" s="3">
-        <v>0.2266690657110298</v>
+        <v>0.2186490552781578</v>
       </c>
       <c r="F41" s="3">
-        <v>0.2266226857203323</v>
+        <v>0.2185779420234487</v>
       </c>
       <c r="G41" s="3">
-        <v>0.226668746166092</v>
+        <v>0.2185873025965624</v>
       </c>
       <c r="H41" s="3">
-        <v>0.2266947877525374</v>
+        <v>0.218576672911541</v>
       </c>
       <c r="I41" s="3">
-        <v>0.2267510752862553</v>
+        <v>0.2185980640136172</v>
       </c>
       <c r="J41" s="3">
-        <v>0.2268393566314901</v>
+        <v>0.2186635447274773</v>
       </c>
       <c r="K41" s="3">
-        <v>0.2268133577466186</v>
+        <v>0.2186205879553978</v>
       </c>
       <c r="L41" s="3">
-        <v>0.2268692058196217</v>
+        <v>0.2186583692499019</v>
       </c>
       <c r="M41" s="3">
-        <v>0.2269018746095992</v>
+        <v>0.2186819942099451</v>
       </c>
       <c r="N41" s="3">
-        <v>0.2269180150405041</v>
+        <v>0.2186948206209756</v>
       </c>
       <c r="O41" s="3">
-        <v>0.2268958509936803</v>
+        <v>0.2186685044862708</v>
       </c>
       <c r="P41" s="3">
-        <v>0.2269329214963391</v>
+        <v>0.2187015457328934</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>10</v>
@@ -2532,46 +2535,46 @@
         <v>0</v>
       </c>
       <c r="D42" s="3">
-        <v>8018.860304005002</v>
+        <v>7038.398971734578</v>
       </c>
       <c r="E42" s="3">
-        <v>8170.876613085665</v>
+        <v>7171.828336127649</v>
       </c>
       <c r="F42" s="3">
-        <v>8360.896999436494</v>
+        <v>7338.615041618989</v>
       </c>
       <c r="G42" s="3">
-        <v>8512.913308517158</v>
+        <v>7472.044406012061</v>
       </c>
       <c r="H42" s="3">
-        <v>8664.929617597822</v>
+        <v>7605.473770405135</v>
       </c>
       <c r="I42" s="3">
-        <v>8854.95000394865</v>
+        <v>7772.260475896474</v>
       </c>
       <c r="J42" s="3">
-        <v>9044.970390299479</v>
+        <v>7939.047181387815</v>
       </c>
       <c r="K42" s="3">
-        <v>9196.986699380142</v>
+        <v>8072.476545780888</v>
       </c>
       <c r="L42" s="3">
-        <v>9425.01116300114</v>
+        <v>8272.620592370497</v>
       </c>
       <c r="M42" s="3">
-        <v>9615.031549351968</v>
+        <v>8439.407297861837</v>
       </c>
       <c r="N42" s="3">
-        <v>9805.051935702799</v>
+        <v>8606.194003353179</v>
       </c>
       <c r="O42" s="3">
-        <v>9995.072322053631</v>
+        <v>8772.980708844521</v>
       </c>
       <c r="P42" s="3">
-        <v>10223.09678567462</v>
+        <v>8973.124755434128</v>
       </c>
       <c r="Q42" s="3">
-        <v>117888.6476920546</v>
+        <v>103474.4720868278</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -2583,46 +2586,46 @@
         <v>0</v>
       </c>
       <c r="D43" s="3">
-        <v>584051.5023487892</v>
+        <v>225195.5175451988</v>
       </c>
       <c r="E43" s="3">
-        <v>597634.0954266679</v>
+        <v>230432.6226043896</v>
       </c>
       <c r="F43" s="3">
-        <v>608500.1698889711</v>
+        <v>234622.3066517421</v>
       </c>
       <c r="G43" s="3">
-        <v>619366.2443512742</v>
+        <v>238811.9906990946</v>
       </c>
       <c r="H43" s="3">
-        <v>632948.837429153</v>
+        <v>244049.0957582853</v>
       </c>
       <c r="I43" s="3">
-        <v>646531.4305070316</v>
+        <v>249286.2008174759</v>
       </c>
       <c r="J43" s="3">
-        <v>657397.5049693347</v>
+        <v>253475.8848648285</v>
       </c>
       <c r="K43" s="3">
-        <v>673696.6166627894</v>
+        <v>259760.4109358573</v>
       </c>
       <c r="L43" s="3">
-        <v>687279.2097406682</v>
+        <v>264997.515995048</v>
       </c>
       <c r="M43" s="3">
-        <v>700861.8028185471</v>
+        <v>270234.6210542386</v>
       </c>
       <c r="N43" s="3">
-        <v>714444.3958964259</v>
+        <v>275471.7261134294</v>
       </c>
       <c r="O43" s="3">
-        <v>730743.5075898806</v>
+        <v>281756.2521844581</v>
       </c>
       <c r="P43" s="3">
-        <v>744326.1006677592</v>
+        <v>286993.3572436487</v>
       </c>
       <c r="Q43" s="3">
-        <v>8597781.418297293</v>
+        <v>3315087.502467695</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -2634,43 +2637,43 @@
         <v>0.18698022</v>
       </c>
       <c r="D44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204751</v>
       </c>
       <c r="E44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204754</v>
       </c>
       <c r="F44" s="3">
-        <v>0.2310431680770575</v>
+        <v>0.08908441396204754</v>
       </c>
       <c r="G44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204751</v>
       </c>
       <c r="H44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204753</v>
       </c>
       <c r="I44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204753</v>
       </c>
       <c r="J44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204754</v>
       </c>
       <c r="K44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204753</v>
       </c>
       <c r="L44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204754</v>
       </c>
       <c r="M44" s="3">
-        <v>0.2310431680770575</v>
+        <v>0.08908441396204754</v>
       </c>
       <c r="N44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204751</v>
       </c>
       <c r="O44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204751</v>
       </c>
       <c r="P44" s="3">
-        <v>0.2310431680770574</v>
+        <v>0.08908441396204751</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>10</v>
@@ -2787,43 +2790,43 @@
         <v>0</v>
       </c>
       <c r="D47" s="3">
-        <v>87.59433119725423</v>
+        <v>87.41250339556255</v>
       </c>
       <c r="E47" s="3">
-        <v>87.10140330778326</v>
+        <v>86.87195576942483</v>
       </c>
       <c r="F47" s="3">
-        <v>86.81353678145324</v>
+        <v>86.55408266294936</v>
       </c>
       <c r="G47" s="3">
-        <v>86.60408205071541</v>
+        <v>86.32321297778509</v>
       </c>
       <c r="H47" s="3">
-        <v>86.41219033357176</v>
+        <v>86.11518711460498</v>
       </c>
       <c r="I47" s="3">
-        <v>86.2511663666846</v>
+        <v>85.94147425202084</v>
       </c>
       <c r="J47" s="3">
-        <v>86.13920908645544</v>
+        <v>85.81912623781379</v>
       </c>
       <c r="K47" s="3">
-        <v>86.01900302164323</v>
+        <v>85.69061246666912</v>
       </c>
       <c r="L47" s="3">
-        <v>85.92545558544077</v>
+        <v>85.59011527217021</v>
       </c>
       <c r="M47" s="3">
-        <v>85.84983329545754</v>
+        <v>85.50862598309401</v>
       </c>
       <c r="N47" s="3">
-        <v>85.78847704659728</v>
+        <v>85.44226962781688</v>
       </c>
       <c r="O47" s="3">
-        <v>85.72713817584935</v>
+        <v>85.37672804431689</v>
       </c>
       <c r="P47" s="3">
-        <v>85.68192474794439</v>
+        <v>85.32782389359143</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>10</v>
@@ -2838,43 +2841,43 @@
         <v>0</v>
       </c>
       <c r="D48" s="3">
-        <v>3.729702466979071</v>
+        <v>3.273673940341664</v>
       </c>
       <c r="E48" s="3">
-        <v>3.721778601630038</v>
+        <v>3.266718921347639</v>
       </c>
       <c r="F48" s="3">
-        <v>3.725437620110343</v>
+        <v>3.269930553790776</v>
       </c>
       <c r="G48" s="3">
-        <v>3.727570149384929</v>
+        <v>3.27180233996542</v>
       </c>
       <c r="H48" s="3">
-        <v>3.725756860950191</v>
+        <v>3.270210761240929</v>
       </c>
       <c r="I48" s="3">
-        <v>3.724847337746009</v>
+        <v>3.269412444903895</v>
       </c>
       <c r="J48" s="3">
-        <v>3.726774827305642</v>
+        <v>3.271104261448919</v>
       </c>
       <c r="K48" s="3">
-        <v>3.724317312568746</v>
+        <v>3.268947225593268</v>
       </c>
       <c r="L48" s="3">
-        <v>3.724435749608356</v>
+        <v>3.269051181405715</v>
       </c>
       <c r="M48" s="3">
-        <v>3.724689556957335</v>
+        <v>3.269273955879437</v>
       </c>
       <c r="N48" s="3">
-        <v>3.725037322056687</v>
+        <v>3.269579199944665</v>
       </c>
       <c r="O48" s="3">
-        <v>3.72416295075683</v>
+        <v>3.268811737509292</v>
       </c>
       <c r="P48" s="3">
-        <v>3.724759800696827</v>
+        <v>3.269335610958223</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>10</v>
@@ -2903,7 +2906,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4422,43 +4425,43 @@
         <v>0</v>
       </c>
       <c r="E31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="F31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="G31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="H31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="I31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="J31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="K31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="L31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="M31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="N31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="O31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="P31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
       <c r="Q31" s="3">
-        <v>0.001503144468540773</v>
+        <v>0.9497986366349089</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -4473,43 +4476,43 @@
         <v>0</v>
       </c>
       <c r="E32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="F32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="G32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="H32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="I32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="J32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="K32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="L32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="M32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="N32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="O32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="P32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="3">
-        <v>4.110920481700742e-07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -4524,43 +4527,43 @@
         <v>0.3538</v>
       </c>
       <c r="E33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="F33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="G33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="H33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="I33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="J33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="K33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="L33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="M33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="N33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="O33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="P33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="3">
-        <v>1.850059426386634e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -4626,43 +4629,43 @@
         <v>0</v>
       </c>
       <c r="E35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="F35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="G35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="H35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="I35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="J35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="K35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="L35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="M35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="N35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="O35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="P35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="3">
-        <v>4.282208835104939e-07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -4728,43 +4731,43 @@
         <v>0.8997000000000001</v>
       </c>
       <c r="E37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="F37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="G37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="H37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="I37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="J37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="K37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="L37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="M37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="N37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="O37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="P37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
       <c r="Q37" s="3">
-        <v>0.95</v>
+        <v>0.949999958929725</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -4779,43 +4782,43 @@
         <v>0</v>
       </c>
       <c r="E38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="F38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="G38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="H38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="I38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="J38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="K38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="L38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="M38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="N38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="O38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="P38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
       <c r="Q38" s="3">
-        <v>0.819800069170432</v>
+        <v>0.01346473922131475</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -5085,43 +5088,43 @@
         <v>0</v>
       </c>
       <c r="E44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="F44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="G44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="H44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="I44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="J44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="K44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="L44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="M44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="N44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="O44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="P44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
       <c r="Q44" s="3">
-        <v>11257.02776814346</v>
+        <v>7113028.621343022</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -5136,43 +5139,43 @@
         <v>0</v>
       </c>
       <c r="E45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="F45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="G45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="H45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="I45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="J45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="K45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="L45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="M45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="N45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="O45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="P45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -5187,43 +5190,43 @@
         <v>3317810.965630114</v>
       </c>
       <c r="E46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="F46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="G46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="H46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="I46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="J46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="K46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="L46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="M46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="N46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="O46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="P46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -5289,43 +5292,43 @@
         <v>0</v>
       </c>
       <c r="E48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="F48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="G48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="H48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="I48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="J48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="K48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="L48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="M48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="N48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="O48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="P48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="3">
-        <v>17.34920139042661</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -5391,43 +5394,43 @@
         <v>3248848.027554</v>
       </c>
       <c r="E50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="F50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="G50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="H50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="I50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="J50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="K50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="L50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="M50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="N50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="O50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="P50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
       <c r="Q50" s="3">
-        <v>3430483.079</v>
+        <v>3430482.930693807</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -5442,43 +5445,43 @@
         <v>0</v>
       </c>
       <c r="E51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="F51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="G51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="H51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="I51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="J51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="K51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="L51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="M51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="N51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="O51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="P51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
       <c r="Q51" s="3">
-        <v>7220308.768811801</v>
+        <v>118589.371147286</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -5817,43 +5820,43 @@
         <v>0</v>
       </c>
       <c r="E59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="F59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="G59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="H59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="J59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="K59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="L59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="M59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="N59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="O59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="P59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="Q59" s="3">
-        <v>0.02245869474512752</v>
+        <v>0.9500000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -5868,43 +5871,43 @@
         <v>0.3538</v>
       </c>
       <c r="E60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="F60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="G60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="H60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="I60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="J60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="K60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="L60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="M60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="N60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="O60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="P60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="Q60" s="3">
-        <v>0.08545010119680628</v>
+        <v>0.9499999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -5970,43 +5973,43 @@
         <v>0</v>
       </c>
       <c r="E62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="F62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="G62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="H62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="I62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="J62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="K62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="L62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="M62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="N62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="O62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="P62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="Q62" s="3">
-        <v>0.0163647526579974</v>
+        <v>0.05000000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -6480,43 +6483,43 @@
         <v>0</v>
       </c>
       <c r="E72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="F72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="G72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="H72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="I72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="J72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="K72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="L72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="M72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="N72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="O72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="P72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
       <c r="Q72" s="3">
-        <v>947817.9396409384</v>
+        <v>40092581.1975</v>
       </c>
     </row>
     <row r="73" spans="1:17">
@@ -6531,43 +6534,43 @@
         <v>3317810.965630114</v>
       </c>
       <c r="E73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="F73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="G73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="H73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="I73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="J73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="K73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="L73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="M73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="N73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="O73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="P73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="Q73" s="3">
-        <v>801320.7539993409</v>
+        <v>8908763.192053726</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -6633,43 +6636,43 @@
         <v>0</v>
       </c>
       <c r="E75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="F75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="G75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="H75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="I75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="J75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="K75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="L75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="M75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="N75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="O75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="P75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
       <c r="Q75" s="3">
-        <v>663011.5449779517</v>
+        <v>38488877.9496</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -6980,19 +6983,70 @@
     </row>
     <row r="82" spans="1:17">
       <c r="A82" s="2"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
-      <c r="N82" s="3"/>
+      <c r="B82" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" s="3">
+        <v>0</v>
+      </c>
+      <c r="E82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="F82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="G82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="H82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="I82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="J82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="K82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="L82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="M82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="N82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="O82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="P82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+      <c r="Q82" s="3">
+        <v>218735.2849374041</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="A83" s="2"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Results and plots updated to include 'Excess budget' program when necessary and results show cost-cov curve for each program
</commit_message>
<xml_diff>
--- a/tests/optim_results.xlsx
+++ b/tests/optim_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="42">
   <si>
     <t>Scenario</t>
   </si>
@@ -89,10 +89,16 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Cost-coverage type</t>
+  </si>
+  <si>
     <t>IFAS (community)</t>
   </si>
   <si>
     <t>Coverage</t>
+  </si>
+  <si>
+    <t>linear</t>
   </si>
   <si>
     <t>IFAS (health facility)</t>
@@ -1344,46 +1350,46 @@
         <v>0</v>
       </c>
       <c r="D18" s="3">
-        <v>1181989.216507733</v>
+        <v>1181989.550008377</v>
       </c>
       <c r="E18" s="3">
-        <v>1199295.611394636</v>
+        <v>1199295.799102015</v>
       </c>
       <c r="F18" s="3">
-        <v>1214453.471733304</v>
+        <v>1214453.538950506</v>
       </c>
       <c r="G18" s="3">
-        <v>1228534.148725318</v>
+        <v>1228534.123469955</v>
       </c>
       <c r="H18" s="3">
-        <v>1243849.139552845</v>
+        <v>1243849.045195602</v>
       </c>
       <c r="I18" s="3">
-        <v>1261229.186969528</v>
+        <v>1261229.041294955</v>
       </c>
       <c r="J18" s="3">
-        <v>1281035.805201516</v>
+        <v>1281035.621161304</v>
       </c>
       <c r="K18" s="3">
-        <v>1302819.912009235</v>
+        <v>1302819.698948233</v>
       </c>
       <c r="L18" s="3">
-        <v>1326178.817375609</v>
+        <v>1326178.58197342</v>
       </c>
       <c r="M18" s="3">
-        <v>1351300.169581505</v>
+        <v>1351299.91647488</v>
       </c>
       <c r="N18" s="3">
-        <v>1377720.500885826</v>
+        <v>1377720.233377207</v>
       </c>
       <c r="O18" s="3">
-        <v>1404953.535417152</v>
+        <v>1404953.255887574</v>
       </c>
       <c r="P18" s="3">
-        <v>1432989.292167476</v>
+        <v>1432989.002264317</v>
       </c>
       <c r="Q18" s="3">
-        <v>16806348.80752169</v>
+        <v>16806347.40810835</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1395,46 +1401,46 @@
         <v>0</v>
       </c>
       <c r="D19" s="3">
-        <v>192227.6281062525</v>
+        <v>192227.5892199371</v>
       </c>
       <c r="E19" s="3">
-        <v>194512.2049523072</v>
+        <v>194512.1696074296</v>
       </c>
       <c r="F19" s="3">
-        <v>197214.5120773835</v>
+        <v>197214.4791904542</v>
       </c>
       <c r="G19" s="3">
-        <v>200140.6906862723</v>
+        <v>200140.6594019948</v>
       </c>
       <c r="H19" s="3">
-        <v>203765.9364240069</v>
+        <v>203765.9061634158</v>
       </c>
       <c r="I19" s="3">
-        <v>207673.4835987023</v>
+        <v>207673.4539085601</v>
       </c>
       <c r="J19" s="3">
-        <v>211212.0562242885</v>
+        <v>211212.0267342256</v>
       </c>
       <c r="K19" s="3">
-        <v>215758.275910671</v>
+        <v>215758.2464368466</v>
       </c>
       <c r="L19" s="3">
-        <v>220103.5072589556</v>
+        <v>220103.4775995899</v>
       </c>
       <c r="M19" s="3">
-        <v>224433.3859193905</v>
+        <v>224433.3559262264</v>
       </c>
       <c r="N19" s="3">
-        <v>228796.1954772036</v>
+        <v>228796.1650600293</v>
       </c>
       <c r="O19" s="3">
-        <v>233710.1750829767</v>
+        <v>233710.144203813</v>
       </c>
       <c r="P19" s="3">
-        <v>238270.3899960906</v>
+        <v>238270.3585711392</v>
       </c>
       <c r="Q19" s="3">
-        <v>2767818.441714501</v>
+        <v>2767818.032023661</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1446,46 +1452,46 @@
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>754750.9718882912</v>
+        <v>754750.6449377933</v>
       </c>
       <c r="E20" s="3">
-        <v>746519.9289767036</v>
+        <v>746519.7574149498</v>
       </c>
       <c r="F20" s="3">
-        <v>741389.9114838012</v>
+        <v>741389.8662866175</v>
       </c>
       <c r="G20" s="3">
-        <v>739499.5810406806</v>
+        <v>739499.6315531841</v>
       </c>
       <c r="H20" s="3">
-        <v>741218.1271043523</v>
+        <v>741218.2484583659</v>
       </c>
       <c r="I20" s="3">
-        <v>746219.6238528547</v>
+        <v>746219.7974655955</v>
       </c>
       <c r="J20" s="3">
-        <v>754116.9500983079</v>
+        <v>754117.1626110387</v>
       </c>
       <c r="K20" s="3">
-        <v>764219.3483201743</v>
+        <v>764219.5901992692</v>
       </c>
       <c r="L20" s="3">
-        <v>775986.3100367729</v>
+        <v>775986.5745328411</v>
       </c>
       <c r="M20" s="3">
-        <v>789309.3616371341</v>
+        <v>789309.644109094</v>
       </c>
       <c r="N20" s="3">
-        <v>803764.4032511218</v>
+        <v>803764.7004274111</v>
       </c>
       <c r="O20" s="3">
-        <v>818958.9810379207</v>
+        <v>818959.2905826672</v>
       </c>
       <c r="P20" s="3">
-        <v>834809.6220345102</v>
+        <v>834809.942348351</v>
       </c>
       <c r="Q20" s="3">
-        <v>10010763.12076263</v>
+        <v>10010764.85092718</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1497,46 +1503,46 @@
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>57261.66778613837</v>
+        <v>57261.62010435046</v>
       </c>
       <c r="E21" s="3">
-        <v>57529.98967720375</v>
+        <v>57529.94205477651</v>
       </c>
       <c r="F21" s="3">
-        <v>57826.47291697245</v>
+        <v>57826.42522034307</v>
       </c>
       <c r="G21" s="3">
-        <v>58186.89274946359</v>
+        <v>58186.84484720241</v>
       </c>
       <c r="H21" s="3">
-        <v>58690.50636606054</v>
+        <v>58690.45809417094</v>
       </c>
       <c r="I21" s="3">
-        <v>59352.23918608791</v>
+        <v>59352.19038876872</v>
       </c>
       <c r="J21" s="3">
-        <v>60171.33411401763</v>
+        <v>60171.28464766655</v>
       </c>
       <c r="K21" s="3">
-        <v>61114.09064316124</v>
+        <v>61114.04039880562</v>
       </c>
       <c r="L21" s="3">
-        <v>62152.6221631123</v>
+        <v>62152.57105861309</v>
       </c>
       <c r="M21" s="3">
-        <v>63289.26955246255</v>
+        <v>63289.21750565879</v>
       </c>
       <c r="N21" s="3">
-        <v>64497.79098383798</v>
+        <v>64497.73793555003</v>
       </c>
       <c r="O21" s="3">
-        <v>65752.20593122006</v>
+        <v>65752.15184441248</v>
       </c>
       <c r="P21" s="3">
-        <v>67049.75133414545</v>
+        <v>67049.69617417727</v>
       </c>
       <c r="Q21" s="3">
-        <v>792874.8334038837</v>
+        <v>792874.1802744959</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1548,46 +1554,46 @@
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>406015.8946034763</v>
+        <v>406015.8959766409</v>
       </c>
       <c r="E22" s="3">
-        <v>407918.4405273829</v>
+        <v>407918.4439121324</v>
       </c>
       <c r="F22" s="3">
-        <v>410020.6654971341</v>
+        <v>410020.6701133842</v>
       </c>
       <c r="G22" s="3">
-        <v>412576.235154453</v>
+        <v>412576.2404493298</v>
       </c>
       <c r="H22" s="3">
-        <v>416147.1254372994</v>
+        <v>416147.1310968702</v>
       </c>
       <c r="I22" s="3">
-        <v>420839.1655629091</v>
+        <v>420839.171419833</v>
       </c>
       <c r="J22" s="3">
-        <v>426646.9873184792</v>
+        <v>426646.9932874238</v>
       </c>
       <c r="K22" s="3">
-        <v>433331.6360612139</v>
+        <v>433331.6421026044</v>
       </c>
       <c r="L22" s="3">
-        <v>440695.3807869467</v>
+        <v>440695.3868861528</v>
       </c>
       <c r="M22" s="3">
-        <v>448754.8195786941</v>
+        <v>448754.8257348076</v>
       </c>
       <c r="N22" s="3">
-        <v>457323.8838249531</v>
+        <v>457323.890044448</v>
       </c>
       <c r="O22" s="3">
-        <v>466218.357680788</v>
+        <v>466218.3639731319</v>
       </c>
       <c r="P22" s="3">
-        <v>475418.6495675868</v>
+        <v>475418.6559428457</v>
       </c>
       <c r="Q22" s="3">
-        <v>5621907.241601316</v>
+        <v>5621907.310939605</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1599,43 +1605,43 @@
         <v>0.3411657413950535</v>
       </c>
       <c r="D23" s="3">
-        <v>0.3319713853578362</v>
+        <v>0.3319714024502247</v>
       </c>
       <c r="E23" s="3">
-        <v>0.3285019485237618</v>
+        <v>0.3285020140334521</v>
       </c>
       <c r="F23" s="3">
-        <v>0.3258082683081363</v>
+        <v>0.3258083688074612</v>
       </c>
       <c r="G23" s="3">
-        <v>0.3238696551527901</v>
+        <v>0.3238697806736184</v>
       </c>
       <c r="H23" s="3">
-        <v>0.322389995205874</v>
+        <v>0.3223901384396054</v>
       </c>
       <c r="I23" s="3">
-        <v>0.3213292496712262</v>
+        <v>0.3213294054261593</v>
       </c>
       <c r="J23" s="3">
-        <v>0.3207016870713299</v>
+        <v>0.3207018516434989</v>
       </c>
       <c r="K23" s="3">
-        <v>0.3200918879032547</v>
+        <v>0.3200920585317318</v>
       </c>
       <c r="L23" s="3">
-        <v>0.319733380517895</v>
+        <v>0.3197335554694546</v>
       </c>
       <c r="M23" s="3">
-        <v>0.3195161392807908</v>
+        <v>0.319516317232391</v>
       </c>
       <c r="N23" s="3">
-        <v>0.3193830631449449</v>
+        <v>0.3193832431661108</v>
       </c>
       <c r="O23" s="3">
-        <v>0.3192075236491017</v>
+        <v>0.319207705065655</v>
       </c>
       <c r="P23" s="3">
-        <v>0.3191693840596564</v>
+        <v>0.3191695665162412</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>10</v>
@@ -1650,43 +1656,43 @@
         <v>0.04535037632743646</v>
       </c>
       <c r="D24" s="3">
-        <v>0.04500834598179335</v>
+        <v>0.04500832176787257</v>
       </c>
       <c r="E24" s="3">
-        <v>0.04507232859671784</v>
+        <v>0.04507230438792185</v>
       </c>
       <c r="F24" s="3">
-        <v>0.04517360941141138</v>
+        <v>0.04517358520342156</v>
       </c>
       <c r="G24" s="3">
-        <v>0.04526371927860786</v>
+        <v>0.04526369506961186</v>
       </c>
       <c r="H24" s="3">
-        <v>0.04536012612486847</v>
+        <v>0.04536010192361426</v>
       </c>
       <c r="I24" s="3">
-        <v>0.0454373888779136</v>
+        <v>0.04543736468114729</v>
       </c>
       <c r="J24" s="3">
-        <v>0.04546426024482765</v>
+        <v>0.04546423604245387</v>
       </c>
       <c r="K24" s="3">
-        <v>0.04552454249857287</v>
+        <v>0.04552451830927448</v>
       </c>
       <c r="L24" s="3">
-        <v>0.04555280305057728</v>
+        <v>0.04555277886076332</v>
       </c>
       <c r="M24" s="3">
-        <v>0.04556401862645677</v>
+        <v>0.04556399443581691</v>
       </c>
       <c r="N24" s="3">
-        <v>0.04556605934333807</v>
+        <v>0.04556603515215701</v>
       </c>
       <c r="O24" s="3">
-        <v>0.04558790309025865</v>
+        <v>0.0455878789058599</v>
       </c>
       <c r="P24" s="3">
-        <v>0.04558337933275754</v>
+        <v>0.0455833551443043</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>10</v>
@@ -1701,43 +1707,43 @@
         <v>0.2195512735036556</v>
       </c>
       <c r="D25" s="3">
-        <v>0.2272073429515667</v>
+        <v>0.2272073430081643</v>
       </c>
       <c r="E25" s="3">
-        <v>0.2268542352049324</v>
+        <v>0.2268542351996665</v>
       </c>
       <c r="F25" s="3">
-        <v>0.226809864282355</v>
+        <v>0.226809864240605</v>
       </c>
       <c r="G25" s="3">
-        <v>0.2268586183348504</v>
+        <v>0.226858618276003</v>
       </c>
       <c r="H25" s="3">
-        <v>0.2268870686948646</v>
+        <v>0.2268870686292221</v>
       </c>
       <c r="I25" s="3">
-        <v>0.2269453753700729</v>
+        <v>0.2269453753021348</v>
       </c>
       <c r="J25" s="3">
-        <v>0.227035111363887</v>
+        <v>0.2270351112952833</v>
       </c>
       <c r="K25" s="3">
-        <v>0.2270100610609329</v>
+        <v>0.2270100609937636</v>
       </c>
       <c r="L25" s="3">
-        <v>0.2270667920616541</v>
+        <v>0.2270667919954893</v>
       </c>
       <c r="M25" s="3">
-        <v>0.2270999830369947</v>
+        <v>0.2270999829719194</v>
       </c>
       <c r="N25" s="3">
-        <v>0.2271164152963361</v>
+        <v>0.2271164152322843</v>
       </c>
       <c r="O25" s="3">
-        <v>0.2270944562298374</v>
+        <v>0.227094456167072</v>
       </c>
       <c r="P25" s="3">
-        <v>0.2271317571742888</v>
+        <v>0.2271317571120332</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>10</v>
@@ -2007,43 +2013,43 @@
         <v>0</v>
       </c>
       <c r="D31" s="3">
-        <v>89.40819911918722</v>
+        <v>89.40818103252887</v>
       </c>
       <c r="E31" s="3">
-        <v>88.90570874909417</v>
+        <v>88.90569168445211</v>
       </c>
       <c r="F31" s="3">
-        <v>88.61219197814009</v>
+        <v>88.61217572349329</v>
       </c>
       <c r="G31" s="3">
-        <v>88.39853842415056</v>
+        <v>88.3985228207233</v>
       </c>
       <c r="H31" s="3">
-        <v>88.20187252198414</v>
+        <v>88.20185746278854</v>
       </c>
       <c r="I31" s="3">
-        <v>88.03641059240977</v>
+        <v>88.03639598614077</v>
       </c>
       <c r="J31" s="3">
-        <v>87.92165700432582</v>
+        <v>87.92164276412606</v>
       </c>
       <c r="K31" s="3">
-        <v>87.79787813743962</v>
+        <v>87.79786421335842</v>
       </c>
       <c r="L31" s="3">
-        <v>87.70148954016372</v>
+        <v>87.70147588112583</v>
       </c>
       <c r="M31" s="3">
-        <v>87.62364057474481</v>
+        <v>87.62362713813819</v>
       </c>
       <c r="N31" s="3">
-        <v>87.56055974963515</v>
+        <v>87.56054650071354</v>
       </c>
       <c r="O31" s="3">
-        <v>87.49733835068869</v>
+        <v>87.49732526643108</v>
       </c>
       <c r="P31" s="3">
-        <v>87.45081964342813</v>
+        <v>87.45080669900983</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>10</v>
@@ -2127,46 +2133,46 @@
         <v>0</v>
       </c>
       <c r="D34" s="3">
-        <v>1207232.89238433</v>
+        <v>1207226.271871526</v>
       </c>
       <c r="E34" s="3">
-        <v>1233725.781504772</v>
+        <v>1233705.290407243</v>
       </c>
       <c r="F34" s="3">
-        <v>1257245.393933501</v>
+        <v>1257213.57507833</v>
       </c>
       <c r="G34" s="3">
-        <v>1278298.590862266</v>
+        <v>1278258.105786648</v>
       </c>
       <c r="H34" s="3">
-        <v>1299195.133325367</v>
+        <v>1299148.069199301</v>
       </c>
       <c r="I34" s="3">
-        <v>1321017.758795508</v>
+        <v>1320965.641265813</v>
       </c>
       <c r="J34" s="3">
-        <v>1344429.304415835</v>
+        <v>1344373.205830219</v>
       </c>
       <c r="K34" s="3">
-        <v>1369208.95822366</v>
+        <v>1369149.640516708</v>
       </c>
       <c r="L34" s="3">
-        <v>1395129.734500986</v>
+        <v>1395067.73535445</v>
       </c>
       <c r="M34" s="3">
-        <v>1422535.739857886</v>
+        <v>1422471.411506272</v>
       </c>
       <c r="N34" s="3">
-        <v>1451045.753453505</v>
+        <v>1450979.344354252</v>
       </c>
       <c r="O34" s="3">
-        <v>1480224.06905238</v>
+        <v>1480155.761370541</v>
       </c>
       <c r="P34" s="3">
-        <v>1510114.350366139</v>
+        <v>1510044.262699601</v>
       </c>
       <c r="Q34" s="3">
-        <v>17569403.46067613</v>
+        <v>17568758.3152409</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2178,46 +2184,46 @@
         <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>187936.8823004595</v>
+        <v>187938.07166741</v>
       </c>
       <c r="E35" s="3">
-        <v>189956.1252965385</v>
+        <v>189957.5310371368</v>
       </c>
       <c r="F35" s="3">
-        <v>192498.3971518383</v>
+        <v>192499.9737664046</v>
       </c>
       <c r="G35" s="3">
-        <v>195295.4943641174</v>
+        <v>195297.203959322</v>
       </c>
       <c r="H35" s="3">
-        <v>198803.196570622</v>
+        <v>198805.0111002464</v>
       </c>
       <c r="I35" s="3">
-        <v>202595.1246588673</v>
+        <v>202597.0264198187</v>
       </c>
       <c r="J35" s="3">
-        <v>206020.7994625776</v>
+        <v>206022.7752060686</v>
       </c>
       <c r="K35" s="3">
-        <v>210456.4985790247</v>
+        <v>210458.5382407019</v>
       </c>
       <c r="L35" s="3">
-        <v>214685.8034842508</v>
+        <v>214687.9036520472</v>
       </c>
       <c r="M35" s="3">
-        <v>218900.1650728914</v>
+        <v>218902.3211580826</v>
       </c>
       <c r="N35" s="3">
-        <v>223147.8227001711</v>
+        <v>223150.0312833457</v>
       </c>
       <c r="O35" s="3">
-        <v>227944.8981198425</v>
+        <v>227947.1576576807</v>
       </c>
       <c r="P35" s="3">
-        <v>232384.4184709669</v>
+        <v>232386.7293101833</v>
       </c>
       <c r="Q35" s="3">
-        <v>2700625.626232169</v>
+        <v>2700650.274458448</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2229,46 +2235,46 @@
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>729915.4085144119</v>
+        <v>729921.9915587573</v>
       </c>
       <c r="E36" s="3">
-        <v>713320.9954999769</v>
+        <v>713341.2436422542</v>
       </c>
       <c r="F36" s="3">
-        <v>700648.0964036074</v>
+        <v>700679.3763864513</v>
       </c>
       <c r="G36" s="3">
-        <v>692497.2052313259</v>
+        <v>692536.8597888374</v>
       </c>
       <c r="H36" s="3">
-        <v>689212.8430939509</v>
+        <v>689258.8219703817</v>
       </c>
       <c r="I36" s="3">
-        <v>690230.3905161001</v>
+        <v>690281.2098516109</v>
       </c>
       <c r="J36" s="3">
-        <v>694886.6295932599</v>
+        <v>694941.2541839224</v>
       </c>
       <c r="K36" s="3">
-        <v>702286.5250977926</v>
+        <v>702344.2234559457</v>
       </c>
       <c r="L36" s="3">
-        <v>711732.7402173075</v>
+        <v>711792.9989156279</v>
       </c>
       <c r="M36" s="3">
-        <v>722975.72564181</v>
+        <v>723038.2109298588</v>
       </c>
       <c r="N36" s="3">
-        <v>735520.1853703291</v>
+        <v>735584.6627451022</v>
       </c>
       <c r="O36" s="3">
-        <v>748930.419567914</v>
+        <v>748996.7175454436</v>
       </c>
       <c r="P36" s="3">
-        <v>763074.7333147051</v>
+        <v>763142.741342625</v>
       </c>
       <c r="Q36" s="3">
-        <v>9295231.89806249</v>
+        <v>9295860.312316818</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2280,46 +2286,46 @@
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>54795.51934068582</v>
+        <v>54795.51828082704</v>
       </c>
       <c r="E37" s="3">
-        <v>55075.51449575907</v>
+        <v>55075.50762335844</v>
       </c>
       <c r="F37" s="3">
-        <v>55382.33214617357</v>
+        <v>55382.31690325748</v>
       </c>
       <c r="G37" s="3">
-        <v>55747.29570848362</v>
+        <v>55747.27221587286</v>
       </c>
       <c r="H37" s="3">
-        <v>56245.48604694257</v>
+        <v>56245.45534881928</v>
       </c>
       <c r="I37" s="3">
-        <v>56891.55900629392</v>
+        <v>56891.52228467356</v>
       </c>
       <c r="J37" s="3">
-        <v>57685.50381605773</v>
+        <v>57685.46212161495</v>
       </c>
       <c r="K37" s="3">
-        <v>58595.75684929314</v>
+        <v>58595.71104327075</v>
       </c>
       <c r="L37" s="3">
-        <v>59596.17207832248</v>
+        <v>59596.12284679809</v>
       </c>
       <c r="M37" s="3">
-        <v>60689.42421646688</v>
+        <v>60689.37208229358</v>
       </c>
       <c r="N37" s="3">
-        <v>61850.71950088612</v>
+        <v>61850.66485878876</v>
       </c>
       <c r="O37" s="3">
-        <v>63055.40873556218</v>
+        <v>63055.35188767327</v>
       </c>
       <c r="P37" s="3">
-        <v>64301.00180873069</v>
+        <v>64300.94298263148</v>
       </c>
       <c r="Q37" s="3">
-        <v>759911.6937496578</v>
+        <v>759911.2204798795</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -2331,46 +2337,46 @@
         <v>0</v>
       </c>
       <c r="D38" s="3">
-        <v>406101.4508199901</v>
+        <v>406101.4429651474</v>
       </c>
       <c r="E38" s="3">
-        <v>408176.5555012845</v>
+        <v>408176.5045684364</v>
       </c>
       <c r="F38" s="3">
-        <v>410450.4474995669</v>
+        <v>410450.3345310173</v>
       </c>
       <c r="G38" s="3">
-        <v>413155.2714328714</v>
+        <v>413155.0973240497</v>
       </c>
       <c r="H38" s="3">
-        <v>416847.4678326319</v>
+        <v>416847.2403221975</v>
       </c>
       <c r="I38" s="3">
-        <v>421635.6543355625</v>
+        <v>421635.3821836879</v>
       </c>
       <c r="J38" s="3">
-        <v>427519.7511193061</v>
+        <v>427519.4421127686</v>
       </c>
       <c r="K38" s="3">
-        <v>434265.8333146751</v>
+        <v>434265.4938363313</v>
       </c>
       <c r="L38" s="3">
-        <v>441680.1270529146</v>
+        <v>441679.7621874342</v>
       </c>
       <c r="M38" s="3">
-        <v>449782.455213218</v>
+        <v>449782.0688355786</v>
       </c>
       <c r="N38" s="3">
-        <v>458389.0658541524</v>
+        <v>458388.660889745</v>
       </c>
       <c r="O38" s="3">
-        <v>467317.2784502856</v>
+        <v>467316.8571382798</v>
       </c>
       <c r="P38" s="3">
-        <v>476548.6382445064</v>
+        <v>476548.2022715561</v>
       </c>
       <c r="Q38" s="3">
-        <v>5631869.996670965</v>
+        <v>5631866.48916623</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -2382,43 +2388,43 @@
         <v>0.3411657413950535</v>
       </c>
       <c r="D39" s="3">
-        <v>0.3160922745145809</v>
+        <v>0.3161054176151433</v>
       </c>
       <c r="E39" s="3">
-        <v>0.3091447504336624</v>
+        <v>0.3091620771754306</v>
       </c>
       <c r="F39" s="3">
-        <v>0.3040247943990836</v>
+        <v>0.3040450986957919</v>
       </c>
       <c r="G39" s="3">
-        <v>0.3003683350575914</v>
+        <v>0.3003907528676086</v>
       </c>
       <c r="H39" s="3">
-        <v>0.2976823746611954</v>
+        <v>0.2977062754668706</v>
       </c>
       <c r="I39" s="3">
-        <v>0.2957749598871964</v>
+        <v>0.2957999038682178</v>
       </c>
       <c r="J39" s="3">
-        <v>0.2945453429856479</v>
+        <v>0.2945710297022983</v>
       </c>
       <c r="K39" s="3">
-        <v>0.2935280423792215</v>
+        <v>0.2935542281530227</v>
       </c>
       <c r="L39" s="3">
-        <v>0.2928803353354885</v>
+        <v>0.292906879828887</v>
       </c>
       <c r="M39" s="3">
-        <v>0.2924586433021583</v>
+        <v>0.2924854401829538</v>
       </c>
       <c r="N39" s="3">
-        <v>0.2921814131874236</v>
+        <v>0.2922083868277446</v>
       </c>
       <c r="O39" s="3">
-        <v>0.2919126266606309</v>
+        <v>0.2919397136431097</v>
       </c>
       <c r="P39" s="3">
-        <v>0.291802715422996</v>
+        <v>0.2918298921938798</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>10</v>
@@ -2433,43 +2439,43 @@
         <v>0.04535037632743646</v>
       </c>
       <c r="D40" s="3">
-        <v>0.04309255930226956</v>
+        <v>0.04309439059285676</v>
       </c>
       <c r="E40" s="3">
-        <v>0.04315490083743631</v>
+        <v>0.04315672694979933</v>
       </c>
       <c r="F40" s="3">
-        <v>0.04325098505820504</v>
+        <v>0.04325281896080743</v>
       </c>
       <c r="G40" s="3">
-        <v>0.04333544178168493</v>
+        <v>0.04333728549069279</v>
       </c>
       <c r="H40" s="3">
-        <v>0.04342675537479384</v>
+        <v>0.04342860862389564</v>
       </c>
       <c r="I40" s="3">
-        <v>0.04349966974085105</v>
+        <v>0.04350153177691553</v>
       </c>
       <c r="J40" s="3">
-        <v>0.04352364469695243</v>
+        <v>0.04352551227631378</v>
       </c>
       <c r="K40" s="3">
-        <v>0.04358165019530206</v>
+        <v>0.04358352226992361</v>
       </c>
       <c r="L40" s="3">
-        <v>0.04360795044569441</v>
+        <v>0.04360982692051079</v>
       </c>
       <c r="M40" s="3">
-        <v>0.04361804436626655</v>
+        <v>0.04361992303049896</v>
       </c>
       <c r="N40" s="3">
-        <v>0.04361953505699136</v>
+        <v>0.04362141456834504</v>
       </c>
       <c r="O40" s="3">
-        <v>0.04364079432591798</v>
+        <v>0.0436426750359843</v>
       </c>
       <c r="P40" s="3">
-        <v>0.04363586234625793</v>
+        <v>0.04363774396195497</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>10</v>
@@ -2484,43 +2490,43 @@
         <v>0.2195512735036556</v>
       </c>
       <c r="D41" s="3">
-        <v>0.2189713419349589</v>
+        <v>0.2214931391111203</v>
       </c>
       <c r="E41" s="3">
-        <v>0.2186490552781578</v>
+        <v>0.2211622499078357</v>
       </c>
       <c r="F41" s="3">
-        <v>0.2185779420234487</v>
+        <v>0.221099068758097</v>
       </c>
       <c r="G41" s="3">
-        <v>0.2185873025965624</v>
+        <v>0.2211198915534594</v>
       </c>
       <c r="H41" s="3">
-        <v>0.218576672911541</v>
+        <v>0.2211206416404842</v>
       </c>
       <c r="I41" s="3">
-        <v>0.2185980640136172</v>
+        <v>0.2211528486601838</v>
       </c>
       <c r="J41" s="3">
-        <v>0.2186635447274773</v>
+        <v>0.2212253693661325</v>
       </c>
       <c r="K41" s="3">
-        <v>0.2186205879553978</v>
+        <v>0.2211876486518216</v>
       </c>
       <c r="L41" s="3">
-        <v>0.2186583692499019</v>
+        <v>0.221231026779599</v>
       </c>
       <c r="M41" s="3">
-        <v>0.2186819942099451</v>
+        <v>0.2212574382311802</v>
       </c>
       <c r="N41" s="3">
-        <v>0.2186948206209756</v>
+        <v>0.2212712679835421</v>
       </c>
       <c r="O41" s="3">
-        <v>0.2186685044862708</v>
+        <v>0.2212462293232448</v>
       </c>
       <c r="P41" s="3">
-        <v>0.2187015457328934</v>
+        <v>0.2212805118243349</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>10</v>
@@ -2790,43 +2796,43 @@
         <v>0</v>
       </c>
       <c r="D47" s="3">
-        <v>87.41250339556255</v>
+        <v>87.41305658949302</v>
       </c>
       <c r="E47" s="3">
-        <v>86.87195576942483</v>
+        <v>86.87255234587285</v>
       </c>
       <c r="F47" s="3">
-        <v>86.55408266294936</v>
+        <v>86.5547157012066</v>
       </c>
       <c r="G47" s="3">
-        <v>86.32321297778509</v>
+        <v>86.32387603498012</v>
       </c>
       <c r="H47" s="3">
-        <v>86.11518711460498</v>
+        <v>86.11587424379643</v>
       </c>
       <c r="I47" s="3">
-        <v>85.94147425202084</v>
+        <v>85.9421809978158</v>
       </c>
       <c r="J47" s="3">
-        <v>85.81912623781379</v>
+        <v>85.81984957227544</v>
       </c>
       <c r="K47" s="3">
-        <v>85.69061246666912</v>
+        <v>85.69134910157517</v>
       </c>
       <c r="L47" s="3">
-        <v>85.59011527217021</v>
+        <v>85.59086316273947</v>
       </c>
       <c r="M47" s="3">
-        <v>85.50862598309401</v>
+        <v>85.50938347635604</v>
       </c>
       <c r="N47" s="3">
-        <v>85.44226962781688</v>
+        <v>85.44303537340139</v>
       </c>
       <c r="O47" s="3">
-        <v>85.37672804431689</v>
+        <v>85.37750069693064</v>
       </c>
       <c r="P47" s="3">
-        <v>85.32782389359143</v>
+        <v>85.32860266851338</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>10</v>
@@ -2906,13 +2912,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:R83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2922,61 +2928,64 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1">
         <v>2017</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>2018</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2019</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2020</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>2021</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>2022</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>2023</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>2024</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>2025</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="1">
         <v>2026</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>2027</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>2028</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="1">
         <v>2029</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="1">
         <v>2030</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
@@ -3017,17 +3026,20 @@
       <c r="Q2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -3068,17 +3080,20 @@
       <c r="Q3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -3119,17 +3134,20 @@
       <c r="Q4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -3170,17 +3188,20 @@
       <c r="Q5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.3538</v>
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E6" s="3">
         <v>0.3538</v>
@@ -3221,17 +3242,20 @@
       <c r="Q6" s="3">
         <v>0.3538</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" s="3">
+        <v>0.3538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.1</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E7" s="3">
         <v>0.1</v>
@@ -3272,17 +3296,20 @@
       <c r="Q7" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -3323,17 +3350,20 @@
       <c r="Q8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -3374,17 +3404,20 @@
       <c r="Q9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.8997000000000001</v>
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E10" s="3">
         <v>0.8997000000000001</v>
@@ -3425,17 +3458,20 @@
       <c r="Q10" s="3">
         <v>0.8997000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10" s="3">
+        <v>0.8997000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -3476,17 +3512,20 @@
       <c r="Q11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -3527,17 +3566,20 @@
       <c r="Q12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
@@ -3578,17 +3620,20 @@
       <c r="Q13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -3629,17 +3674,20 @@
       <c r="Q14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
@@ -3680,17 +3728,20 @@
       <c r="Q15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -3731,17 +3782,20 @@
       <c r="Q16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -3782,17 +3836,20 @@
       <c r="Q17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -3833,17 +3890,20 @@
       <c r="Q18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="3">
-        <v>3317810.965630114</v>
+        <v>40</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E19" s="3">
         <v>3317810.965630114</v>
@@ -3884,17 +3944,20 @@
       <c r="Q19" s="3">
         <v>3317810.965630114</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R19" s="3">
+        <v>3317810.965630114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="3">
-        <v>4095441.930000001</v>
+        <v>40</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E20" s="3">
         <v>4095441.930000001</v>
@@ -3935,17 +3998,20 @@
       <c r="Q20" s="3">
         <v>4095441.930000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="R20" s="3">
+        <v>4095441.930000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
@@ -3986,17 +4052,20 @@
       <c r="Q21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -4037,17 +4106,20 @@
       <c r="Q22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="3">
-        <v>3248848.027554</v>
+        <v>40</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E23" s="3">
         <v>3248848.027554</v>
@@ -4088,17 +4160,20 @@
       <c r="Q23" s="3">
         <v>3248848.027554</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23" s="3">
+        <v>3248848.027554</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -4139,17 +4214,20 @@
       <c r="Q24" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="R24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -4190,17 +4268,20 @@
       <c r="Q25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="R25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
@@ -4241,17 +4322,20 @@
       <c r="Q26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="R26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
@@ -4292,8 +4376,11 @@
       <c r="Q27" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4309,18 +4396,18 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:18">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
@@ -4361,17 +4448,20 @@
       <c r="Q29" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="3">
-        <v>0</v>
+      <c r="D30" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
@@ -4412,68 +4502,74 @@
       <c r="Q30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="R30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0</v>
       </c>
       <c r="F31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="G31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="H31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="I31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="J31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="K31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="L31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="M31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="N31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="O31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="P31" s="3">
-        <v>0.9497986366349089</v>
+        <v>0.9497792690463163</v>
       </c>
       <c r="Q31" s="3">
-        <v>0.9497986366349089</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
+        <v>0.9497792690463163</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0.9497792690463163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
@@ -4514,21 +4610,24 @@
       <c r="Q32" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="3">
+        <v>26</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="3">
         <v>0.3538</v>
       </c>
-      <c r="E33" s="3">
-        <v>0</v>
-      </c>
       <c r="F33" s="3">
         <v>0</v>
       </c>
@@ -4565,21 +4664,24 @@
       <c r="Q33" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="3">
+        <v>26</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="3">
         <v>0.1</v>
       </c>
-      <c r="E34" s="3">
-        <v>0</v>
-      </c>
       <c r="F34" s="3">
         <v>0</v>
       </c>
@@ -4616,17 +4718,20 @@
       <c r="Q34" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="R34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
@@ -4667,17 +4772,20 @@
       <c r="Q35" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="R35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="2"/>
       <c r="B36" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
@@ -4718,119 +4826,128 @@
       <c r="Q36" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:17">
+      <c r="R36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37" s="2"/>
       <c r="B37" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="3">
+        <v>26</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="3">
         <v>0.8997000000000001</v>
       </c>
-      <c r="E37" s="3">
-        <v>0.949999958929725</v>
-      </c>
       <c r="F37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="G37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="H37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="I37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="J37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="K37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="L37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="M37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="N37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="O37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="P37" s="3">
-        <v>0.949999958929725</v>
+        <v>0.9499996680977512</v>
       </c>
       <c r="Q37" s="3">
-        <v>0.949999958929725</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
+        <v>0.9499996680977512</v>
+      </c>
+      <c r="R37" s="3">
+        <v>0.9499996680977512</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="2"/>
       <c r="B38" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0</v>
       </c>
       <c r="F38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="G38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="H38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="I38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="J38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="K38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="L38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="M38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="N38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="O38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="P38" s="3">
-        <v>0.01346473922131475</v>
+        <v>0.01348132683736274</v>
       </c>
       <c r="Q38" s="3">
-        <v>0.01346473922131475</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
+        <v>0.01348132683736274</v>
+      </c>
+      <c r="R38" s="3">
+        <v>0.01348132683736274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="2"/>
       <c r="B39" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
@@ -4871,17 +4988,20 @@
       <c r="Q39" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="R39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="2"/>
       <c r="B40" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
@@ -4922,17 +5042,20 @@
       <c r="Q40" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:17">
+      <c r="R40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="2"/>
       <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
@@ -4973,17 +5096,20 @@
       <c r="Q41" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="R41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="2"/>
       <c r="B42" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
@@ -5024,17 +5150,20 @@
       <c r="Q42" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="R42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="2"/>
       <c r="B43" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E43" s="3">
         <v>0</v>
@@ -5075,68 +5204,74 @@
       <c r="Q43" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="R43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="2"/>
       <c r="B44" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E44" s="3">
-        <v>7113028.621343022</v>
+        <v>0</v>
       </c>
       <c r="F44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="G44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="H44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="I44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="J44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="K44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="L44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="M44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="N44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="O44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="P44" s="3">
-        <v>7113028.621343022</v>
+        <v>7112883.577744651</v>
       </c>
       <c r="Q44" s="3">
-        <v>7113028.621343022</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
+        <v>7112883.577744651</v>
+      </c>
+      <c r="R44" s="3">
+        <v>7112883.577744651</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="2"/>
       <c r="B45" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
@@ -5177,21 +5312,24 @@
       <c r="Q45" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="R45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" s="2"/>
       <c r="B46" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="3">
+        <v>40</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="3">
         <v>3317810.965630114</v>
       </c>
-      <c r="E46" s="3">
-        <v>0</v>
-      </c>
       <c r="F46" s="3">
         <v>0</v>
       </c>
@@ -5228,21 +5366,24 @@
       <c r="Q46" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:17">
+      <c r="R46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" s="2"/>
       <c r="B47" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D47" s="3">
+        <v>40</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="3">
         <v>4095441.930000001</v>
       </c>
-      <c r="E47" s="3">
-        <v>0</v>
-      </c>
       <c r="F47" s="3">
         <v>0</v>
       </c>
@@ -5279,17 +5420,20 @@
       <c r="Q47" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="R47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" s="2"/>
       <c r="B48" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E48" s="3">
         <v>0</v>
@@ -5330,17 +5474,20 @@
       <c r="Q48" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:17">
+      <c r="R48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49" s="2"/>
       <c r="B49" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E49" s="3">
         <v>0</v>
@@ -5381,119 +5528,128 @@
       <c r="Q49" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:17">
+      <c r="R49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50" s="2"/>
       <c r="B50" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" s="3">
+        <v>40</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="3">
         <v>3248848.027554</v>
       </c>
-      <c r="E50" s="3">
-        <v>3430482.930693807</v>
-      </c>
       <c r="F50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="G50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="H50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="I50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="J50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="K50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="L50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="M50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="N50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="O50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="P50" s="3">
-        <v>3430482.930693807</v>
+        <v>3430481.880489422</v>
       </c>
       <c r="Q50" s="3">
-        <v>3430482.930693807</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17">
+        <v>3430481.880489422</v>
+      </c>
+      <c r="R50" s="3">
+        <v>3430481.880489422</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51" s="2"/>
       <c r="B51" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E51" s="3">
-        <v>118589.371147286</v>
+        <v>0</v>
       </c>
       <c r="F51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="G51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="H51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="I51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="J51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="K51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="L51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="M51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="N51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="O51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="P51" s="3">
-        <v>118589.371147286</v>
+        <v>118735.4649500423</v>
       </c>
       <c r="Q51" s="3">
-        <v>118589.371147286</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17">
+        <v>118735.4649500423</v>
+      </c>
+      <c r="R51" s="3">
+        <v>118735.4649500423</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" s="2"/>
       <c r="B52" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E52" s="3">
         <v>0</v>
@@ -5534,17 +5690,20 @@
       <c r="Q52" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:17">
+      <c r="R52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53" s="2"/>
       <c r="B53" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
@@ -5585,17 +5744,20 @@
       <c r="Q53" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="R53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54" s="2"/>
       <c r="B54" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D54" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
@@ -5636,8 +5798,11 @@
       <c r="Q54" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:17">
+      <c r="R54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -5653,18 +5818,18 @@
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:18">
       <c r="A56" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D56" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E56" s="3">
         <v>0</v>
@@ -5705,17 +5870,20 @@
       <c r="Q56" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:17">
+      <c r="R56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
       <c r="A57" s="2"/>
       <c r="B57" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D57" s="3">
-        <v>0</v>
+      <c r="D57" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
@@ -5756,20 +5924,23 @@
       <c r="Q57" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:17">
+      <c r="R57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58" s="2"/>
       <c r="B58" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="F58" s="3">
         <v>0.9500000000000001</v>
@@ -5807,71 +5978,77 @@
       <c r="Q58" s="3">
         <v>0.9500000000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:17">
+      <c r="R58" s="3">
+        <v>0.9500000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59" s="2"/>
       <c r="B59" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="F59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="G59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="H59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="I59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="J59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="K59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="L59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="M59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="N59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="O59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="P59" s="3">
-        <v>0.9500000000000001</v>
+        <v>0.6594636339893744</v>
       </c>
       <c r="Q59" s="3">
-        <v>0.9500000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17">
+        <v>0.6594636339893744</v>
+      </c>
+      <c r="R59" s="3">
+        <v>0.6594636339893744</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60" s="2"/>
       <c r="B60" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="3">
+        <v>26</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="3">
         <v>0.3538</v>
-      </c>
-      <c r="E60" s="3">
-        <v>0.9499999999999998</v>
       </c>
       <c r="F60" s="3">
         <v>0.9499999999999998</v>
@@ -5909,21 +6086,24 @@
       <c r="Q60" s="3">
         <v>0.9499999999999998</v>
       </c>
-    </row>
-    <row r="61" spans="1:17">
+      <c r="R60" s="3">
+        <v>0.9499999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61" s="2"/>
       <c r="B61" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61" s="3">
+        <v>26</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="3">
         <v>0.1</v>
       </c>
-      <c r="E61" s="3">
-        <v>0</v>
-      </c>
       <c r="F61" s="3">
         <v>0</v>
       </c>
@@ -5960,68 +6140,74 @@
       <c r="Q61" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:17">
+      <c r="R61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62" s="2"/>
       <c r="B62" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0</v>
       </c>
       <c r="F62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="G62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="H62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="I62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="J62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="K62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="L62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="M62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="N62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="O62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="P62" s="3">
-        <v>0.05000000000000002</v>
+        <v>0.3405363660106256</v>
       </c>
       <c r="Q62" s="3">
-        <v>0.05000000000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17">
+        <v>0.3405363660106256</v>
+      </c>
+      <c r="R62" s="3">
+        <v>0.3405363660106256</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63" s="2"/>
       <c r="B63" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E63" s="3">
         <v>0</v>
@@ -6062,20 +6248,23 @@
       <c r="Q63" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:17">
+      <c r="R63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64" s="2"/>
       <c r="B64" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D64" s="3">
+        <v>26</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="3">
         <v>0.8997000000000001</v>
-      </c>
-      <c r="E64" s="3">
-        <v>0.95</v>
       </c>
       <c r="F64" s="3">
         <v>0.95</v>
@@ -6113,20 +6302,23 @@
       <c r="Q64" s="3">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="65" spans="1:17">
+      <c r="R64" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65" s="2"/>
       <c r="B65" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D65" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="F65" s="3">
         <v>0.95</v>
@@ -6164,17 +6356,20 @@
       <c r="Q65" s="3">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="66" spans="1:17">
+      <c r="R65" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66" s="2"/>
       <c r="B66" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D66" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E66" s="3">
         <v>0</v>
@@ -6215,17 +6410,20 @@
       <c r="Q66" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:17">
+      <c r="R66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67" s="2"/>
       <c r="B67" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D67" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E67" s="3">
         <v>0</v>
@@ -6266,17 +6464,20 @@
       <c r="Q67" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:17">
+      <c r="R67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68" s="2"/>
       <c r="B68" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" s="3">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E68" s="3">
         <v>0</v>
@@ -6317,17 +6518,20 @@
       <c r="Q68" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:17">
+      <c r="R68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69" s="2"/>
       <c r="B69" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D69" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E69" s="3">
         <v>0</v>
@@ -6368,17 +6572,20 @@
       <c r="Q69" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:17">
+      <c r="R69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
       <c r="A70" s="2"/>
       <c r="B70" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D70" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E70" s="3">
         <v>0</v>
@@ -6419,20 +6626,23 @@
       <c r="Q70" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:17">
+      <c r="R70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71" s="2"/>
       <c r="B71" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D71" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="F71" s="3">
         <v>7114536.62875</v>
@@ -6470,71 +6680,77 @@
       <c r="Q71" s="3">
         <v>7114536.62875</v>
       </c>
-    </row>
-    <row r="72" spans="1:17">
+      <c r="R71" s="3">
+        <v>7114536.62875</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72" s="2"/>
       <c r="B72" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D72" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E72" s="3">
-        <v>40092581.1975</v>
+        <v>0</v>
       </c>
       <c r="F72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="G72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="H72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="I72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="J72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="K72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="L72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="M72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="N72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="O72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="P72" s="3">
-        <v>40092581.1975</v>
+        <v>27831157.15001833</v>
       </c>
       <c r="Q72" s="3">
-        <v>40092581.1975</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17">
+        <v>27831157.15001833</v>
+      </c>
+      <c r="R72" s="3">
+        <v>27831157.15001833</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73" s="2"/>
       <c r="B73" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D73" s="3">
+        <v>40</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" s="3">
         <v>3317810.965630114</v>
-      </c>
-      <c r="E73" s="3">
-        <v>8908763.192053726</v>
       </c>
       <c r="F73" s="3">
         <v>8908763.192053726</v>
@@ -6572,21 +6788,24 @@
       <c r="Q73" s="3">
         <v>8908763.192053726</v>
       </c>
-    </row>
-    <row r="74" spans="1:17">
+      <c r="R73" s="3">
+        <v>8908763.192053726</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74" s="2"/>
       <c r="B74" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D74" s="3">
+        <v>40</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="3">
         <v>4095441.930000001</v>
       </c>
-      <c r="E74" s="3">
-        <v>0</v>
-      </c>
       <c r="F74" s="3">
         <v>0</v>
       </c>
@@ -6623,20 +6842,23 @@
       <c r="Q74" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:17">
+      <c r="R74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
       <c r="A75" s="2"/>
       <c r="B75" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D75" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="F75" s="3">
         <v>38488877.9496</v>
@@ -6674,17 +6896,20 @@
       <c r="Q75" s="3">
         <v>38488877.9496</v>
       </c>
-    </row>
-    <row r="76" spans="1:17">
+      <c r="R75" s="3">
+        <v>38488877.9496</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
       <c r="A76" s="2"/>
       <c r="B76" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E76" s="3">
         <v>0</v>
@@ -6725,20 +6950,23 @@
       <c r="Q76" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:17">
+      <c r="R76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
       <c r="A77" s="2"/>
       <c r="B77" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D77" s="3">
+        <v>40</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E77" s="3">
         <v>3248848.027554</v>
-      </c>
-      <c r="E77" s="3">
-        <v>3430483.079</v>
       </c>
       <c r="F77" s="3">
         <v>3430483.079</v>
@@ -6776,20 +7004,23 @@
       <c r="Q77" s="3">
         <v>3430483.079</v>
       </c>
-    </row>
-    <row r="78" spans="1:17">
+      <c r="R77" s="3">
+        <v>3430483.079</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
       <c r="A78" s="2"/>
       <c r="B78" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D78" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E78" s="3">
-        <v>8367031.899999999</v>
+        <v>0</v>
       </c>
       <c r="F78" s="3">
         <v>8367031.899999999</v>
@@ -6827,17 +7058,20 @@
       <c r="Q78" s="3">
         <v>8367031.899999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:17">
+      <c r="R78" s="3">
+        <v>8367031.899999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
       <c r="A79" s="2"/>
       <c r="B79" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D79" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E79" s="3">
         <v>0</v>
@@ -6878,17 +7112,20 @@
       <c r="Q79" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:17">
+      <c r="R79" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
       <c r="A80" s="2"/>
       <c r="B80" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D80" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
@@ -6929,17 +7166,20 @@
       <c r="Q80" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:17">
+      <c r="R80" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
       <c r="A81" s="2"/>
       <c r="B81" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D81" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E81" s="3">
         <v>0</v>
@@ -6980,59 +7220,65 @@
       <c r="Q81" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:17">
+      <c r="R81" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
       <c r="A82" s="2"/>
       <c r="B82" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D82" s="3">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E82" s="3">
-        <v>218735.2849374041</v>
+        <v>0</v>
       </c>
       <c r="F82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="G82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="H82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="I82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="J82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="K82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="L82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="M82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="N82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="O82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="P82" s="3">
-        <v>218735.2849374041</v>
+        <v>12480159.33241911</v>
       </c>
       <c r="Q82" s="3">
-        <v>218735.2849374041</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17">
+        <v>12480159.33241911</v>
+      </c>
+      <c r="R82" s="3">
+        <v>12480159.33241911</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>

</xml_diff>

<commit_message>
Changed name of excess budget program and added it to all result outputs
</commit_message>
<xml_diff>
--- a/tests/optim_results.xlsx
+++ b/tests/optim_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="42">
   <si>
     <t>Scenario</t>
   </si>
@@ -137,10 +137,10 @@
     <t>Mg for pre-eclampsia</t>
   </si>
   <si>
-    <t>Budget</t>
+    <t>Excess budget not allocated</t>
   </si>
   <si>
-    <t>Excess budget</t>
+    <t>Budget</t>
   </si>
 </sst>
 </file>
@@ -1350,46 +1350,46 @@
         <v>0</v>
       </c>
       <c r="D18" s="3">
-        <v>1181989.550008377</v>
+        <v>1180061.77530382</v>
       </c>
       <c r="E18" s="3">
-        <v>1199295.799102015</v>
+        <v>1187680.377362981</v>
       </c>
       <c r="F18" s="3">
-        <v>1214453.538950506</v>
+        <v>1195111.467673738</v>
       </c>
       <c r="G18" s="3">
-        <v>1228534.123469955</v>
+        <v>1203352.535325252</v>
       </c>
       <c r="H18" s="3">
-        <v>1243849.045195602</v>
+        <v>1214267.152756223</v>
       </c>
       <c r="I18" s="3">
-        <v>1261229.041294955</v>
+        <v>1228285.735530704</v>
       </c>
       <c r="J18" s="3">
-        <v>1281035.621161304</v>
+        <v>1245457.430955918</v>
       </c>
       <c r="K18" s="3">
-        <v>1302819.698948233</v>
+        <v>1265121.303143498</v>
       </c>
       <c r="L18" s="3">
-        <v>1326178.58197342</v>
+        <v>1286722.732570882</v>
       </c>
       <c r="M18" s="3">
-        <v>1351299.91647488</v>
+        <v>1310325.029411871</v>
       </c>
       <c r="N18" s="3">
-        <v>1377720.233377207</v>
+        <v>1335394.459510236</v>
       </c>
       <c r="O18" s="3">
-        <v>1404953.255887574</v>
+        <v>1361399.645883647</v>
       </c>
       <c r="P18" s="3">
-        <v>1432989.002264317</v>
+        <v>1388288.027833981</v>
       </c>
       <c r="Q18" s="3">
-        <v>16806347.40810835</v>
+        <v>16401467.67326275</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1401,46 +1401,46 @@
         <v>0</v>
       </c>
       <c r="D19" s="3">
-        <v>192227.5892199371</v>
+        <v>193046.1828064489</v>
       </c>
       <c r="E19" s="3">
-        <v>194512.1696074296</v>
+        <v>195483.6889367717</v>
       </c>
       <c r="F19" s="3">
-        <v>197214.4791904542</v>
+        <v>198319.2190378476</v>
       </c>
       <c r="G19" s="3">
-        <v>200140.6594019948</v>
+        <v>201348.7760479938</v>
       </c>
       <c r="H19" s="3">
-        <v>203765.9061634158</v>
+        <v>205056.5170700764</v>
       </c>
       <c r="I19" s="3">
-        <v>207673.4539085601</v>
+        <v>209032.3059244996</v>
       </c>
       <c r="J19" s="3">
-        <v>211212.0267342256</v>
+        <v>212626.6188075776</v>
       </c>
       <c r="K19" s="3">
-        <v>215758.2464368466</v>
+        <v>217222.5137611368</v>
       </c>
       <c r="L19" s="3">
-        <v>220103.4775995899</v>
+        <v>221613.4888302841</v>
       </c>
       <c r="M19" s="3">
-        <v>224433.3559262264</v>
+        <v>225984.4337903127</v>
       </c>
       <c r="N19" s="3">
-        <v>228796.1650600293</v>
+        <v>230385.4751795551</v>
       </c>
       <c r="O19" s="3">
-        <v>233710.144203813</v>
+        <v>235337.5263599583</v>
       </c>
       <c r="P19" s="3">
-        <v>238270.3585711392</v>
+        <v>239934.6971021361</v>
       </c>
       <c r="Q19" s="3">
-        <v>2767818.032023661</v>
+        <v>2785391.443654598</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1452,46 +1452,46 @@
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>754750.6449377933</v>
+        <v>756704.2526550088</v>
       </c>
       <c r="E20" s="3">
-        <v>746519.7574149498</v>
+        <v>758084.290070044</v>
       </c>
       <c r="F20" s="3">
-        <v>741389.8662866175</v>
+        <v>760484.8851974065</v>
       </c>
       <c r="G20" s="3">
-        <v>739499.6315531841</v>
+        <v>764210.5609399129</v>
       </c>
       <c r="H20" s="3">
-        <v>741218.2484583659</v>
+        <v>770124.4033163897</v>
       </c>
       <c r="I20" s="3">
-        <v>746219.7974655955</v>
+        <v>778313.4329099529</v>
       </c>
       <c r="J20" s="3">
-        <v>754117.1626110387</v>
+        <v>788702.0003378052</v>
       </c>
       <c r="K20" s="3">
-        <v>764219.5901992692</v>
+        <v>800806.5512454719</v>
       </c>
       <c r="L20" s="3">
-        <v>775986.5745328411</v>
+        <v>814233.5590806929</v>
       </c>
       <c r="M20" s="3">
-        <v>789309.644109094</v>
+        <v>828994.029105781</v>
       </c>
       <c r="N20" s="3">
-        <v>803764.7004274111</v>
+        <v>844730.3374080983</v>
       </c>
       <c r="O20" s="3">
-        <v>818959.2905826672</v>
+        <v>861092.3705980873</v>
       </c>
       <c r="P20" s="3">
-        <v>834809.942348351</v>
+        <v>878036.959959254</v>
       </c>
       <c r="Q20" s="3">
-        <v>10010764.85092718</v>
+        <v>10404517.6328239</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1503,46 +1503,46 @@
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>57261.62010435046</v>
+        <v>56927.75535314713</v>
       </c>
       <c r="E21" s="3">
-        <v>57529.94205477651</v>
+        <v>57192.25418217611</v>
       </c>
       <c r="F21" s="3">
-        <v>57826.42522034307</v>
+        <v>57481.23889961266</v>
       </c>
       <c r="G21" s="3">
-        <v>58186.84484720241</v>
+        <v>57832.97980712261</v>
       </c>
       <c r="H21" s="3">
-        <v>58690.45809417094</v>
+        <v>58327.62212790841</v>
       </c>
       <c r="I21" s="3">
-        <v>59352.19038876872</v>
+        <v>58980.37496723716</v>
       </c>
       <c r="J21" s="3">
-        <v>60171.28464766655</v>
+        <v>59790.45934424435</v>
       </c>
       <c r="K21" s="3">
-        <v>61114.04039880562</v>
+        <v>60724.23502587765</v>
       </c>
       <c r="L21" s="3">
-        <v>62152.57105861309</v>
+        <v>61753.83296290377</v>
       </c>
       <c r="M21" s="3">
-        <v>63289.21750565879</v>
+        <v>62881.4375239583</v>
       </c>
       <c r="N21" s="3">
-        <v>64497.73793555003</v>
+        <v>64080.84884114604</v>
       </c>
       <c r="O21" s="3">
-        <v>65752.15184441248</v>
+        <v>65326.15708978368</v>
       </c>
       <c r="P21" s="3">
-        <v>67049.69617417727</v>
+        <v>66614.5484758369</v>
       </c>
       <c r="Q21" s="3">
-        <v>792874.1802744959</v>
+        <v>787913.7446009548</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1554,46 +1554,46 @@
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>406015.8959766409</v>
+        <v>406021.3115784898</v>
       </c>
       <c r="E22" s="3">
-        <v>407918.4439121324</v>
+        <v>407907.7755854951</v>
       </c>
       <c r="F22" s="3">
-        <v>410020.6701133842</v>
+        <v>409968.8783511293</v>
       </c>
       <c r="G22" s="3">
-        <v>412576.2404493298</v>
+        <v>412477.5721107386</v>
       </c>
       <c r="H22" s="3">
-        <v>416147.1310968702</v>
+        <v>416005.4702792472</v>
       </c>
       <c r="I22" s="3">
-        <v>420839.171419833</v>
+        <v>420661.04755112</v>
       </c>
       <c r="J22" s="3">
-        <v>426646.9932874238</v>
+        <v>426438.7480629587</v>
       </c>
       <c r="K22" s="3">
-        <v>433331.6421026044</v>
+        <v>433098.6422503357</v>
       </c>
       <c r="L22" s="3">
-        <v>440695.3868861528</v>
+        <v>440441.961905161</v>
       </c>
       <c r="M22" s="3">
-        <v>448754.8257348076</v>
+        <v>448484.2864264973</v>
       </c>
       <c r="N22" s="3">
-        <v>457323.890044448</v>
+        <v>457038.7525758416</v>
       </c>
       <c r="O22" s="3">
-        <v>466218.3639731319</v>
+        <v>465920.5657668725</v>
       </c>
       <c r="P22" s="3">
-        <v>475418.6559428457</v>
+        <v>475109.6573997089</v>
       </c>
       <c r="Q22" s="3">
-        <v>5621907.310939605</v>
+        <v>5619574.669843597</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1605,43 +1605,43 @@
         <v>0.3411657413950535</v>
       </c>
       <c r="D23" s="3">
-        <v>0.3319714024502247</v>
+        <v>0.3396999578817883</v>
       </c>
       <c r="E23" s="3">
-        <v>0.3285020140334521</v>
+        <v>0.3390023485584416</v>
       </c>
       <c r="F23" s="3">
-        <v>0.3258083688074612</v>
+        <v>0.3382904200009951</v>
       </c>
       <c r="G23" s="3">
-        <v>0.3238697806736184</v>
+        <v>0.3377594792705149</v>
       </c>
       <c r="H23" s="3">
-        <v>0.3223901384396054</v>
+        <v>0.3372665988682505</v>
       </c>
       <c r="I23" s="3">
-        <v>0.3213294054261593</v>
+        <v>0.3368996694024569</v>
       </c>
       <c r="J23" s="3">
-        <v>0.3207018516434989</v>
+        <v>0.336766881059452</v>
       </c>
       <c r="K23" s="3">
-        <v>0.3200920585317318</v>
+        <v>0.3364879183400866</v>
       </c>
       <c r="L23" s="3">
-        <v>0.3197335554694546</v>
+        <v>0.3363677172720747</v>
       </c>
       <c r="M23" s="3">
-        <v>0.319516317232391</v>
+        <v>0.336318334927727</v>
       </c>
       <c r="N23" s="3">
-        <v>0.3193832431661108</v>
+        <v>0.3363028363071687</v>
       </c>
       <c r="O23" s="3">
-        <v>0.319207705065655</v>
+        <v>0.336201919520525</v>
       </c>
       <c r="P23" s="3">
-        <v>0.3191695665162412</v>
+        <v>0.3362236656576046</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>10</v>
@@ -1656,43 +1656,43 @@
         <v>0.04535037632743646</v>
       </c>
       <c r="D24" s="3">
-        <v>0.04500832176787257</v>
+        <v>0.04485531813194561</v>
       </c>
       <c r="E24" s="3">
-        <v>0.04507230438792185</v>
+        <v>0.04491946606493546</v>
       </c>
       <c r="F24" s="3">
-        <v>0.04517358520342156</v>
+        <v>0.04502160278517826</v>
       </c>
       <c r="G24" s="3">
-        <v>0.04526369506961186</v>
+        <v>0.04511271700727327</v>
       </c>
       <c r="H24" s="3">
-        <v>0.04536010192361426</v>
+        <v>0.04521001513581416</v>
       </c>
       <c r="I24" s="3">
-        <v>0.04543736468114729</v>
+        <v>0.04528802032346177</v>
       </c>
       <c r="J24" s="3">
-        <v>0.04546423604245387</v>
+        <v>0.04531548357533249</v>
       </c>
       <c r="K24" s="3">
-        <v>0.04552451830927448</v>
+        <v>0.04537618416370487</v>
       </c>
       <c r="L24" s="3">
-        <v>0.04555277886076332</v>
+        <v>0.0454047868156461</v>
       </c>
       <c r="M24" s="3">
-        <v>0.04556399443581691</v>
+        <v>0.0454162533300552</v>
       </c>
       <c r="N24" s="3">
-        <v>0.04556603515215701</v>
+        <v>0.04541847112852658</v>
       </c>
       <c r="O24" s="3">
-        <v>0.0455878789058599</v>
+        <v>0.0454404344901984</v>
       </c>
       <c r="P24" s="3">
-        <v>0.0455833551443043</v>
+        <v>0.0454360160442354</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>10</v>
@@ -1707,43 +1707,43 @@
         <v>0.2195512735036556</v>
       </c>
       <c r="D25" s="3">
-        <v>0.2272073430081643</v>
+        <v>0.2269481916179022</v>
       </c>
       <c r="E25" s="3">
-        <v>0.2268542351996665</v>
+        <v>0.2265928848011396</v>
       </c>
       <c r="F25" s="3">
-        <v>0.226809864240605</v>
+        <v>0.2265471599834154</v>
       </c>
       <c r="G25" s="3">
-        <v>0.226858618276003</v>
+        <v>0.2265951685283872</v>
       </c>
       <c r="H25" s="3">
-        <v>0.2268870686292221</v>
+        <v>0.2266230973377116</v>
       </c>
       <c r="I25" s="3">
-        <v>0.2269453753021348</v>
+        <v>0.2266809048625142</v>
       </c>
       <c r="J25" s="3">
-        <v>0.2270351112952833</v>
+        <v>0.2267704288030534</v>
       </c>
       <c r="K25" s="3">
-        <v>0.2270100609937636</v>
+        <v>0.2267452171342221</v>
       </c>
       <c r="L25" s="3">
-        <v>0.2270667919954893</v>
+        <v>0.2268016806669623</v>
       </c>
       <c r="M25" s="3">
-        <v>0.2270999829719194</v>
+        <v>0.226834809933337</v>
       </c>
       <c r="N25" s="3">
-        <v>0.2271164152322843</v>
+        <v>0.2268513055537821</v>
       </c>
       <c r="O25" s="3">
-        <v>0.227094456167072</v>
+        <v>0.2268293288600996</v>
       </c>
       <c r="P25" s="3">
-        <v>0.2271317571120332</v>
+        <v>0.2268666030143205</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>10</v>
@@ -1758,46 +1758,46 @@
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>8115.766821694776</v>
+        <v>7937.243903323931</v>
       </c>
       <c r="E26" s="3">
-        <v>8269.620221158184</v>
+        <v>8087.712982059928</v>
       </c>
       <c r="F26" s="3">
-        <v>8461.936970487444</v>
+        <v>8275.799330479927</v>
       </c>
       <c r="G26" s="3">
-        <v>8615.79036995085</v>
+        <v>8426.268409215925</v>
       </c>
       <c r="H26" s="3">
-        <v>8769.643769414261</v>
+        <v>8576.737487951923</v>
       </c>
       <c r="I26" s="3">
-        <v>8961.960518743519</v>
+        <v>8764.823836371921</v>
       </c>
       <c r="J26" s="3">
-        <v>9154.277268072779</v>
+        <v>8952.910184791919</v>
       </c>
       <c r="K26" s="3">
-        <v>9308.130667536187</v>
+        <v>9103.379263527919</v>
       </c>
       <c r="L26" s="3">
-        <v>9538.910766731298</v>
+        <v>9329.082881631917</v>
       </c>
       <c r="M26" s="3">
-        <v>9731.227516060559</v>
+        <v>9517.169230051915</v>
       </c>
       <c r="N26" s="3">
-        <v>9923.544265389817</v>
+        <v>9705.255578471913</v>
       </c>
       <c r="O26" s="3">
-        <v>10115.86101471908</v>
+        <v>9893.341926891913</v>
       </c>
       <c r="P26" s="3">
-        <v>10346.64111391419</v>
+        <v>10119.04554499591</v>
       </c>
       <c r="Q26" s="3">
-        <v>119313.3112838729</v>
+        <v>116688.770559767</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1809,46 +1809,46 @@
         <v>0</v>
       </c>
       <c r="D27" s="3">
-        <v>619519.9932467644</v>
+        <v>554179.3055792259</v>
       </c>
       <c r="E27" s="3">
-        <v>633927.4349501774</v>
+        <v>567067.1964066497</v>
       </c>
       <c r="F27" s="3">
-        <v>645453.388312908</v>
+        <v>577377.5090685887</v>
       </c>
       <c r="G27" s="3">
-        <v>656979.3416756385</v>
+        <v>587687.8217305279</v>
       </c>
       <c r="H27" s="3">
-        <v>671386.7833790516</v>
+        <v>600575.7125579518</v>
       </c>
       <c r="I27" s="3">
-        <v>685794.2250824647</v>
+        <v>613463.6033853756</v>
       </c>
       <c r="J27" s="3">
-        <v>697320.1784451953</v>
+        <v>623773.9160473146</v>
       </c>
       <c r="K27" s="3">
-        <v>714609.1084892909</v>
+        <v>639239.3850402232</v>
       </c>
       <c r="L27" s="3">
-        <v>729016.5501927041</v>
+        <v>652127.2758676471</v>
       </c>
       <c r="M27" s="3">
-        <v>743423.9918961172</v>
+        <v>665015.1666950709</v>
       </c>
       <c r="N27" s="3">
-        <v>757831.4335995305</v>
+        <v>677903.0575224949</v>
       </c>
       <c r="O27" s="3">
-        <v>775120.3636436262</v>
+        <v>693368.5265154035</v>
       </c>
       <c r="P27" s="3">
-        <v>789527.8053470392</v>
+        <v>706256.4173428274</v>
       </c>
       <c r="Q27" s="3">
-        <v>9119910.598260507</v>
+        <v>8158034.893759303</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1860,43 +1860,43 @@
         <v>0.18698022</v>
       </c>
       <c r="D28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="E28" s="3">
-        <v>0.245074041161066</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="F28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="G28" s="3">
-        <v>0.245074041161066</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="H28" s="3">
-        <v>0.245074041161066</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="I28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="J28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="K28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="L28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="M28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="N28" s="3">
-        <v>0.245074041161066</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="O28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="P28" s="3">
-        <v>0.2450740411610661</v>
+        <v>0.2192261160682784</v>
       </c>
       <c r="Q28" s="3" t="s">
         <v>10</v>
@@ -2013,43 +2013,43 @@
         <v>0</v>
       </c>
       <c r="D31" s="3">
-        <v>89.40818103252887</v>
+        <v>89.78892223555765</v>
       </c>
       <c r="E31" s="3">
-        <v>88.90569168445211</v>
+        <v>89.31721189499325</v>
       </c>
       <c r="F31" s="3">
-        <v>88.61217572349329</v>
+        <v>89.0514553537281</v>
       </c>
       <c r="G31" s="3">
-        <v>88.3985228207233</v>
+        <v>88.86108983416707</v>
       </c>
       <c r="H31" s="3">
-        <v>88.20185746278854</v>
+        <v>88.68342713385164</v>
       </c>
       <c r="I31" s="3">
-        <v>88.03639598614077</v>
+        <v>88.53362958936951</v>
       </c>
       <c r="J31" s="3">
-        <v>87.92164276412606</v>
+        <v>88.43208178945098</v>
       </c>
       <c r="K31" s="3">
-        <v>87.79786421335842</v>
+        <v>88.31903800824418</v>
       </c>
       <c r="L31" s="3">
-        <v>87.70147588112583</v>
+        <v>88.23176160031588</v>
       </c>
       <c r="M31" s="3">
-        <v>87.62362713813819</v>
+        <v>88.1616678682895</v>
       </c>
       <c r="N31" s="3">
-        <v>87.56054650071354</v>
+        <v>88.10523341695286</v>
       </c>
       <c r="O31" s="3">
-        <v>87.49732526643108</v>
+        <v>88.04762181087727</v>
       </c>
       <c r="P31" s="3">
-        <v>87.45080669900983</v>
+        <v>88.00604877265714</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>10</v>
@@ -2064,43 +2064,43 @@
         <v>0</v>
       </c>
       <c r="D32" s="3">
-        <v>3.774775265904547</v>
+        <v>3.691741350383224</v>
       </c>
       <c r="E32" s="3">
-        <v>3.766755642035163</v>
+        <v>3.683898134571002</v>
       </c>
       <c r="F32" s="3">
-        <v>3.770458879110835</v>
+        <v>3.68751991136021</v>
       </c>
       <c r="G32" s="3">
-        <v>3.772617179626973</v>
+        <v>3.689630735634692</v>
       </c>
       <c r="H32" s="3">
-        <v>3.770781977920135</v>
+        <v>3.687835902949254</v>
       </c>
       <c r="I32" s="3">
-        <v>3.769861463287852</v>
+        <v>3.686935636922206</v>
       </c>
       <c r="J32" s="3">
-        <v>3.771812246220114</v>
+        <v>3.688843508387217</v>
       </c>
       <c r="K32" s="3">
-        <v>3.769325032849459</v>
+        <v>3.686411006370314</v>
       </c>
       <c r="L32" s="3">
-        <v>3.769444901179881</v>
+        <v>3.686528237951229</v>
       </c>
       <c r="M32" s="3">
-        <v>3.769701775746073</v>
+        <v>3.686779462035067</v>
       </c>
       <c r="N32" s="3">
-        <v>3.770053743525541</v>
+        <v>3.687123687562134</v>
       </c>
       <c r="O32" s="3">
-        <v>3.769168805602171</v>
+        <v>3.686258215661399</v>
       </c>
       <c r="P32" s="3">
-        <v>3.769772868368814</v>
+        <v>3.68684899082992</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>10</v>
@@ -2133,46 +2133,46 @@
         <v>0</v>
       </c>
       <c r="D34" s="3">
-        <v>1207226.271871526</v>
+        <v>1206807.199857086</v>
       </c>
       <c r="E34" s="3">
-        <v>1233705.290407243</v>
+        <v>1232433.682366206</v>
       </c>
       <c r="F34" s="3">
-        <v>1257213.57507833</v>
+        <v>1255261.496116258</v>
       </c>
       <c r="G34" s="3">
-        <v>1278258.105786648</v>
+        <v>1275790.176515055</v>
       </c>
       <c r="H34" s="3">
-        <v>1299148.069199301</v>
+        <v>1296289.899447877</v>
       </c>
       <c r="I34" s="3">
-        <v>1320965.641265813</v>
+        <v>1317807.946471761</v>
       </c>
       <c r="J34" s="3">
-        <v>1344373.205830219</v>
+        <v>1340979.350390371</v>
       </c>
       <c r="K34" s="3">
-        <v>1369149.640516708</v>
+        <v>1365564.51098741</v>
       </c>
       <c r="L34" s="3">
-        <v>1395067.73535445</v>
+        <v>1391322.953505152</v>
       </c>
       <c r="M34" s="3">
-        <v>1422471.411506272</v>
+        <v>1418587.630066806</v>
       </c>
       <c r="N34" s="3">
-        <v>1450979.344354252</v>
+        <v>1446971.122552851</v>
       </c>
       <c r="O34" s="3">
-        <v>1480155.761370541</v>
+        <v>1476033.781276616</v>
       </c>
       <c r="P34" s="3">
-        <v>1510044.262699601</v>
+        <v>1505815.459182271</v>
       </c>
       <c r="Q34" s="3">
-        <v>17568758.3152409</v>
+        <v>17529665.20873572</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2184,46 +2184,46 @@
         <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>187938.07166741</v>
+        <v>188004.4376505825</v>
       </c>
       <c r="E35" s="3">
-        <v>189957.5310371368</v>
+        <v>190036.9280916817</v>
       </c>
       <c r="F35" s="3">
-        <v>192499.9737664046</v>
+        <v>192589.4745570173</v>
       </c>
       <c r="G35" s="3">
-        <v>195297.203959322</v>
+        <v>195394.5097848852</v>
       </c>
       <c r="H35" s="3">
-        <v>198805.0111002464</v>
+        <v>198908.4489834378</v>
       </c>
       <c r="I35" s="3">
-        <v>202597.0264198187</v>
+        <v>202705.5361634689</v>
       </c>
       <c r="J35" s="3">
-        <v>206022.7752060686</v>
+        <v>206135.5753546733</v>
       </c>
       <c r="K35" s="3">
-        <v>210458.5382407019</v>
+        <v>210575.0373820596</v>
       </c>
       <c r="L35" s="3">
-        <v>214687.9036520472</v>
+        <v>214807.8847752757</v>
       </c>
       <c r="M35" s="3">
-        <v>218902.3211580826</v>
+        <v>219025.5197194554</v>
       </c>
       <c r="N35" s="3">
-        <v>223150.0312833457</v>
+        <v>223276.2486170708</v>
       </c>
       <c r="O35" s="3">
-        <v>227947.1576576807</v>
+        <v>228076.2990200812</v>
       </c>
       <c r="P35" s="3">
-        <v>232386.7293101833</v>
+        <v>232518.8082038981</v>
       </c>
       <c r="Q35" s="3">
-        <v>2700650.274458448</v>
+        <v>2702054.708303588</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2235,46 +2235,46 @@
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>729921.9915587573</v>
+        <v>730338.8521129875</v>
       </c>
       <c r="E36" s="3">
-        <v>713341.2436422542</v>
+        <v>714598.7999059015</v>
       </c>
       <c r="F36" s="3">
-        <v>700679.3763864513</v>
+        <v>702600.5322435468</v>
       </c>
       <c r="G36" s="3">
-        <v>692536.8597888374</v>
+        <v>694957.2712383333</v>
       </c>
       <c r="H36" s="3">
-        <v>689258.8219703817</v>
+        <v>692054.9686687358</v>
       </c>
       <c r="I36" s="3">
-        <v>690281.2098516109</v>
+        <v>693364.7363856043</v>
       </c>
       <c r="J36" s="3">
-        <v>694941.2541839224</v>
+        <v>698250.8976012106</v>
       </c>
       <c r="K36" s="3">
-        <v>702344.2234559457</v>
+        <v>705836.8240566417</v>
       </c>
       <c r="L36" s="3">
-        <v>711792.9989156279</v>
+        <v>715438.3140236837</v>
       </c>
       <c r="M36" s="3">
-        <v>723038.2109298588</v>
+        <v>726816.6420595975</v>
       </c>
       <c r="N36" s="3">
-        <v>735584.6627451022</v>
+        <v>739482.4484212475</v>
       </c>
       <c r="O36" s="3">
-        <v>748996.7175454436</v>
+        <v>753003.7871870417</v>
       </c>
       <c r="P36" s="3">
-        <v>763142.741342625</v>
+        <v>767252.6215521985</v>
       </c>
       <c r="Q36" s="3">
-        <v>9295860.312316818</v>
+        <v>9333996.69545673</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2286,46 +2286,46 @@
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>54795.51828082704</v>
+        <v>54795.45572593094</v>
       </c>
       <c r="E37" s="3">
-        <v>55075.50762335844</v>
+        <v>55075.1101450449</v>
       </c>
       <c r="F37" s="3">
-        <v>55382.31690325748</v>
+        <v>55381.44219087949</v>
       </c>
       <c r="G37" s="3">
-        <v>55747.27221587286</v>
+        <v>55745.92809382576</v>
       </c>
       <c r="H37" s="3">
-        <v>56245.45534881928</v>
+        <v>56243.70092175632</v>
       </c>
       <c r="I37" s="3">
-        <v>56891.52228467356</v>
+        <v>56889.4243098687</v>
       </c>
       <c r="J37" s="3">
-        <v>57685.46212161495</v>
+        <v>57683.0800419834</v>
       </c>
       <c r="K37" s="3">
-        <v>58595.71104327075</v>
+        <v>58593.09370587098</v>
       </c>
       <c r="L37" s="3">
-        <v>59596.12284679809</v>
+        <v>59593.30926162189</v>
       </c>
       <c r="M37" s="3">
-        <v>60689.37208229358</v>
+        <v>60686.39207042173</v>
       </c>
       <c r="N37" s="3">
-        <v>61850.66485878876</v>
+        <v>61847.54098601426</v>
       </c>
       <c r="O37" s="3">
-        <v>63055.35188767327</v>
+        <v>63052.10145098239</v>
       </c>
       <c r="P37" s="3">
-        <v>64300.94298263148</v>
+        <v>64297.57903553089</v>
       </c>
       <c r="Q37" s="3">
-        <v>759911.2204798795</v>
+        <v>759884.1579397317</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -2337,46 +2337,46 @@
         <v>0</v>
       </c>
       <c r="D38" s="3">
-        <v>406101.4429651474</v>
+        <v>406100.9793572763</v>
       </c>
       <c r="E38" s="3">
-        <v>408176.5045684364</v>
+        <v>408173.5587706459</v>
       </c>
       <c r="F38" s="3">
-        <v>410450.3345310173</v>
+        <v>410443.8518483085</v>
       </c>
       <c r="G38" s="3">
-        <v>413155.0973240497</v>
+        <v>413145.1357447094</v>
       </c>
       <c r="H38" s="3">
-        <v>416847.2403221975</v>
+        <v>416834.2378836005</v>
       </c>
       <c r="I38" s="3">
-        <v>421635.3821836879</v>
+        <v>421619.8336384368</v>
       </c>
       <c r="J38" s="3">
-        <v>427519.4421127686</v>
+        <v>427501.7880051702</v>
       </c>
       <c r="K38" s="3">
-        <v>434265.4938363313</v>
+        <v>434246.0961825064</v>
       </c>
       <c r="L38" s="3">
-        <v>441679.7621874342</v>
+        <v>441658.9100988727</v>
       </c>
       <c r="M38" s="3">
-        <v>449782.0688355786</v>
+        <v>449759.9833227634</v>
       </c>
       <c r="N38" s="3">
-        <v>458388.660889745</v>
+        <v>458365.5091926508</v>
       </c>
       <c r="O38" s="3">
-        <v>467316.8571382798</v>
+        <v>467292.7674486145</v>
       </c>
       <c r="P38" s="3">
-        <v>476548.2022715561</v>
+        <v>476523.2713316824</v>
       </c>
       <c r="Q38" s="3">
-        <v>5631866.48916623</v>
+        <v>5631665.922825238</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -2388,43 +2388,43 @@
         <v>0.3411657413950535</v>
       </c>
       <c r="D39" s="3">
-        <v>0.3161054176151433</v>
+        <v>0.3168983388592954</v>
       </c>
       <c r="E39" s="3">
-        <v>0.3091620771754306</v>
+        <v>0.310202827513652</v>
       </c>
       <c r="F39" s="3">
-        <v>0.3040450986957919</v>
+        <v>0.3052617413385249</v>
       </c>
       <c r="G39" s="3">
-        <v>0.3003907528676086</v>
+        <v>0.3017321412515211</v>
       </c>
       <c r="H39" s="3">
-        <v>0.2977062754668706</v>
+        <v>0.2991351181434045</v>
       </c>
       <c r="I39" s="3">
-        <v>0.2957999038682178</v>
+        <v>0.2972902402932081</v>
       </c>
       <c r="J39" s="3">
-        <v>0.2945710297022983</v>
+        <v>0.29610520043921</v>
       </c>
       <c r="K39" s="3">
-        <v>0.2935542281530227</v>
+        <v>0.2951177802412621</v>
       </c>
       <c r="L39" s="3">
-        <v>0.292906879828887</v>
+        <v>0.2944915711939547</v>
       </c>
       <c r="M39" s="3">
-        <v>0.2924854401829538</v>
+        <v>0.2940850260741387</v>
       </c>
       <c r="N39" s="3">
-        <v>0.2922083868277446</v>
+        <v>0.2938184134584395</v>
       </c>
       <c r="O39" s="3">
-        <v>0.2919397136431097</v>
+        <v>0.2935563979747829</v>
       </c>
       <c r="P39" s="3">
-        <v>0.2918298921938798</v>
+        <v>0.2934518869183853</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>10</v>
@@ -2439,43 +2439,43 @@
         <v>0.04535037632743646</v>
       </c>
       <c r="D40" s="3">
-        <v>0.04309439059285676</v>
+        <v>0.04319229172717397</v>
       </c>
       <c r="E40" s="3">
-        <v>0.04315672694979933</v>
+        <v>0.04325435573370881</v>
       </c>
       <c r="F40" s="3">
-        <v>0.04325281896080743</v>
+        <v>0.04335086913239638</v>
       </c>
       <c r="G40" s="3">
-        <v>0.04333728549069279</v>
+        <v>0.04343586439016794</v>
       </c>
       <c r="H40" s="3">
-        <v>0.04342860862389564</v>
+        <v>0.04352770133551669</v>
       </c>
       <c r="I40" s="3">
-        <v>0.04350153177691553</v>
+        <v>0.04360109731709898</v>
       </c>
       <c r="J40" s="3">
-        <v>0.04352551227631378</v>
+        <v>0.04362537655872793</v>
       </c>
       <c r="K40" s="3">
-        <v>0.04358352226992361</v>
+        <v>0.04368362878155485</v>
       </c>
       <c r="L40" s="3">
-        <v>0.04360982692051079</v>
+        <v>0.04371017010267909</v>
       </c>
       <c r="M40" s="3">
-        <v>0.04361992303049896</v>
+        <v>0.04372038433513564</v>
       </c>
       <c r="N40" s="3">
-        <v>0.04362141456834504</v>
+        <v>0.04372192196876753</v>
       </c>
       <c r="O40" s="3">
-        <v>0.0436426750359843</v>
+        <v>0.04374324715404206</v>
       </c>
       <c r="P40" s="3">
-        <v>0.04363774396195497</v>
+        <v>0.04373836493574863</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>10</v>
@@ -2490,43 +2490,43 @@
         <v>0.2195512735036556</v>
       </c>
       <c r="D41" s="3">
-        <v>0.2214931391111203</v>
+        <v>0.221713351846098</v>
       </c>
       <c r="E41" s="3">
-        <v>0.2211622499078357</v>
+        <v>0.221381617155138</v>
       </c>
       <c r="F41" s="3">
-        <v>0.221099068758097</v>
+        <v>0.2213191334944583</v>
       </c>
       <c r="G41" s="3">
-        <v>0.2211198915534594</v>
+        <v>0.221340990030081</v>
       </c>
       <c r="H41" s="3">
-        <v>0.2211206416404842</v>
+        <v>0.2213427689022676</v>
       </c>
       <c r="I41" s="3">
-        <v>0.2211528486601838</v>
+        <v>0.2213759513607752</v>
       </c>
       <c r="J41" s="3">
-        <v>0.2212253693661325</v>
+        <v>0.2214491127061101</v>
       </c>
       <c r="K41" s="3">
-        <v>0.2211876486518216</v>
+        <v>0.2214118667023336</v>
       </c>
       <c r="L41" s="3">
-        <v>0.221231026779599</v>
+        <v>0.2214557488246147</v>
       </c>
       <c r="M41" s="3">
-        <v>0.2212574382311802</v>
+        <v>0.2214824147065543</v>
       </c>
       <c r="N41" s="3">
-        <v>0.2212712679835421</v>
+        <v>0.2214963402495495</v>
       </c>
       <c r="O41" s="3">
-        <v>0.2212462293232448</v>
+        <v>0.2214714181406096</v>
       </c>
       <c r="P41" s="3">
-        <v>0.2212805118243349</v>
+        <v>0.2215058143940009</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>10</v>
@@ -2796,43 +2796,43 @@
         <v>0</v>
       </c>
       <c r="D47" s="3">
-        <v>87.41305658949302</v>
+        <v>87.44392448864301</v>
       </c>
       <c r="E47" s="3">
-        <v>86.87255234587285</v>
+        <v>86.90606109017568</v>
       </c>
       <c r="F47" s="3">
-        <v>86.5547157012066</v>
+        <v>86.59041582690159</v>
       </c>
       <c r="G47" s="3">
-        <v>86.32387603498012</v>
+        <v>86.36136979528374</v>
       </c>
       <c r="H47" s="3">
-        <v>86.11587424379643</v>
+        <v>86.15480348817897</v>
       </c>
       <c r="I47" s="3">
-        <v>85.9421809978158</v>
+        <v>85.98227799934267</v>
       </c>
       <c r="J47" s="3">
-        <v>85.81984957227544</v>
+        <v>85.86093191160916</v>
       </c>
       <c r="K47" s="3">
-        <v>85.69134910157517</v>
+        <v>85.73322229263022</v>
       </c>
       <c r="L47" s="3">
-        <v>85.59086316273947</v>
+        <v>85.63340469981352</v>
       </c>
       <c r="M47" s="3">
-        <v>85.50938347635604</v>
+        <v>85.5524948055336</v>
       </c>
       <c r="N47" s="3">
-        <v>85.44303537340139</v>
+        <v>85.4866361967814</v>
       </c>
       <c r="O47" s="3">
-        <v>85.37750069693064</v>
+        <v>85.42151159113419</v>
       </c>
       <c r="P47" s="3">
-        <v>85.32860266851338</v>
+        <v>85.37297656567416</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>10</v>
@@ -2912,7 +2912,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3681,10 +3681,10 @@
     <row r="15" spans="1:18">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>27</v>
@@ -3735,10 +3735,10 @@
     <row r="16" spans="1:18">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>27</v>
@@ -3789,10 +3789,10 @@
     <row r="17" spans="1:18">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>27</v>
@@ -3843,10 +3843,10 @@
     <row r="18" spans="1:18">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>27</v>
@@ -3897,172 +3897,172 @@
     <row r="19" spans="1:18">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="F19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="G19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="H19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="I19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="J19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="K19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="L19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="M19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="N19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="O19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="P19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="R19" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="F20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="G20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="H20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="I20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="J20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="K20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="L20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="M20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="N20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="O20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="P20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="Q20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="R20" s="3">
-        <v>4095441.930000001</v>
+        <v>3317810.965630114</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="F21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="G21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="H21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="I21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="J21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="K21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="L21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="M21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="N21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="O21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="P21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="Q21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="R21" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>27</v>
@@ -4113,118 +4113,118 @@
     <row r="23" spans="1:18">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="F23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="G23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="H23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="I23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="K23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="L23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="M23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="N23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="O23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="P23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="R23" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="G24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="H24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="I24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="J24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="K24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="L24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="M24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="N24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="O24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="P24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="Q24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="R24" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>27</v>
@@ -4275,10 +4275,10 @@
     <row r="26" spans="1:18">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>27</v>
@@ -4329,10 +4329,10 @@
     <row r="27" spans="1:18">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>27</v>
@@ -4382,29 +4382,65 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>27</v>
@@ -4454,62 +4490,26 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="2"/>
-      <c r="B30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
-        <v>0</v>
-      </c>
-      <c r="J30" s="3">
-        <v>0</v>
-      </c>
-      <c r="K30" s="3">
-        <v>0</v>
-      </c>
-      <c r="L30" s="3">
-        <v>0</v>
-      </c>
-      <c r="M30" s="3">
-        <v>0</v>
-      </c>
-      <c r="N30" s="3">
-        <v>0</v>
-      </c>
-      <c r="O30" s="3">
-        <v>0</v>
-      </c>
-      <c r="P30" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="3">
-        <v>0</v>
-      </c>
-      <c r="R30" s="3">
-        <v>0</v>
-      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B31" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>26</v>
@@ -4521,49 +4521,49 @@
         <v>0</v>
       </c>
       <c r="F31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="G31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="H31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="I31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="J31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="K31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="L31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="M31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="N31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="O31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="P31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
       <c r="R31" s="3">
-        <v>0.9497792690463163</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>26</v>
@@ -4617,7 +4617,7 @@
     <row r="33" spans="1:18">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>26</v>
@@ -4626,52 +4626,52 @@
         <v>27</v>
       </c>
       <c r="E33" s="3">
-        <v>0.3538</v>
+        <v>0</v>
       </c>
       <c r="F33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="G33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="H33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="I33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="J33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="K33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="L33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="M33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="N33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="O33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="P33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="Q33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
       <c r="R33" s="3">
-        <v>0</v>
+        <v>0.07715504719778994</v>
       </c>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>26</v>
@@ -4680,52 +4680,52 @@
         <v>27</v>
       </c>
       <c r="E34" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="G34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="H34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="I34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="J34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="K34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="L34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="M34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="N34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="O34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="P34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="Q34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
       <c r="R34" s="3">
-        <v>0</v>
+        <v>0.02957133392176595</v>
       </c>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>26</v>
@@ -4734,52 +4734,52 @@
         <v>27</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="F35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="G35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="H35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="I35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="J35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="K35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="L35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="M35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="N35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="O35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="P35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="Q35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
       <c r="R35" s="3">
-        <v>0</v>
+        <v>0.1574177032093245</v>
       </c>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="2"/>
       <c r="B36" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>26</v>
@@ -4788,7 +4788,7 @@
         <v>27</v>
       </c>
       <c r="E36" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F36" s="3">
         <v>0</v>
@@ -4833,7 +4833,7 @@
     <row r="37" spans="1:18">
       <c r="A37" s="2"/>
       <c r="B37" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>26</v>
@@ -4842,52 +4842,52 @@
         <v>27</v>
       </c>
       <c r="E37" s="3">
-        <v>0.8997000000000001</v>
+        <v>0</v>
       </c>
       <c r="F37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="G37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="H37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="I37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="J37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="K37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="L37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="M37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="N37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="O37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="P37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="Q37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
       <c r="R37" s="3">
-        <v>0.9499996680977512</v>
+        <v>0.04255021520138764</v>
       </c>
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="2"/>
       <c r="B38" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>26</v>
@@ -4899,49 +4899,49 @@
         <v>0</v>
       </c>
       <c r="F38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="G38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="H38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="I38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="J38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="K38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="L38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="M38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="N38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="O38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="P38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
       <c r="R38" s="3">
-        <v>0.01348132683736274</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="2"/>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>26</v>
@@ -4950,52 +4950,52 @@
         <v>27</v>
       </c>
       <c r="E39" s="3">
-        <v>0</v>
+        <v>0.8997000000000001</v>
       </c>
       <c r="F39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="G39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="H39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="I39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="J39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="K39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="L39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="M39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="N39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="O39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="P39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="Q39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
       <c r="R39" s="3">
-        <v>0</v>
+        <v>0.726433402072844</v>
       </c>
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="2"/>
       <c r="B40" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>26</v>
@@ -5007,49 +5007,49 @@
         <v>0</v>
       </c>
       <c r="F40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="G40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="H40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="I40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="J40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="K40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="L40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="M40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="N40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="O40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="P40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="Q40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
       <c r="R40" s="3">
-        <v>0</v>
+        <v>0.3420995428128968</v>
       </c>
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="2"/>
       <c r="B41" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>26</v>
@@ -5103,10 +5103,10 @@
     <row r="42" spans="1:18">
       <c r="A42" s="2"/>
       <c r="B42" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>27</v>
@@ -5157,10 +5157,10 @@
     <row r="43" spans="1:18">
       <c r="A43" s="2"/>
       <c r="B43" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>27</v>
@@ -5211,10 +5211,10 @@
     <row r="44" spans="1:18">
       <c r="A44" s="2"/>
       <c r="B44" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>27</v>
@@ -5223,52 +5223,52 @@
         <v>0</v>
       </c>
       <c r="F44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="G44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="H44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="I44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="J44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="K44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="L44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="M44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="N44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="O44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="P44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
       <c r="R44" s="3">
-        <v>7112883.577744651</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="2"/>
       <c r="B45" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>27</v>
@@ -5319,16 +5319,16 @@
     <row r="46" spans="1:18">
       <c r="A46" s="2"/>
       <c r="B46" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E46" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="F46" s="3">
         <v>0</v>
@@ -5373,64 +5373,64 @@
     <row r="47" spans="1:18">
       <c r="A47" s="2"/>
       <c r="B47" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E47" s="3">
-        <v>4095441.930000001</v>
+        <v>0</v>
       </c>
       <c r="F47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="G47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="H47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="I47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="J47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="K47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="L47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="M47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="N47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="O47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="P47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="Q47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
       <c r="R47" s="3">
-        <v>0</v>
+        <v>577813.0625069595</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="2"/>
       <c r="B48" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>27</v>
@@ -5439,160 +5439,160 @@
         <v>0</v>
       </c>
       <c r="F48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="G48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="H48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="I48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="J48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="K48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="L48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="M48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="N48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="O48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="P48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="Q48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
       <c r="R48" s="3">
-        <v>0</v>
+        <v>1247990.638291355</v>
       </c>
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="2"/>
       <c r="B49" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E49" s="3">
-        <v>0</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="F49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="G49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="H49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="I49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="J49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="K49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="L49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="M49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="N49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="O49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="P49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="Q49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
       <c r="R49" s="3">
-        <v>0</v>
+        <v>1476207.410661967</v>
       </c>
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="2"/>
       <c r="B50" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E50" s="3">
-        <v>3248848.027554</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="F50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="G50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="H50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="I50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="J50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="K50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="L50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="M50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="N50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="O50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="P50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
       <c r="R50" s="3">
-        <v>3430481.880489422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="2"/>
       <c r="B51" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>27</v>
@@ -5601,52 +5601,52 @@
         <v>0</v>
       </c>
       <c r="F51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="G51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="H51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="I51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="J51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="K51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="L51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="M51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="N51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="O51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="P51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="Q51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
       <c r="R51" s="3">
-        <v>118735.4649500423</v>
+        <v>1723905.30485834</v>
       </c>
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="2"/>
       <c r="B52" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>27</v>
@@ -5697,64 +5697,64 @@
     <row r="53" spans="1:18">
       <c r="A53" s="2"/>
       <c r="B53" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E53" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="F53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="G53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="H53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="I53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="J53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="K53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="L53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="M53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="N53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="O53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="P53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="Q53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
       <c r="R53" s="3">
-        <v>0</v>
+        <v>2623176.3092961</v>
       </c>
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="2"/>
       <c r="B54" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>27</v>
@@ -5763,70 +5763,106 @@
         <v>0</v>
       </c>
       <c r="F54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="G54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="H54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="I54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="J54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="K54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="L54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="M54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="N54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="O54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="P54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="Q54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
       <c r="R54" s="3">
-        <v>0</v>
+        <v>3013008.197569393</v>
       </c>
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="2"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0</v>
+      </c>
+      <c r="L55" s="3">
+        <v>0</v>
+      </c>
+      <c r="M55" s="3">
+        <v>0</v>
+      </c>
+      <c r="N55" s="3">
+        <v>0</v>
+      </c>
+      <c r="O55" s="3">
+        <v>0</v>
+      </c>
+      <c r="P55" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="3">
+        <v>0</v>
+      </c>
+      <c r="R55" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A56" s="2"/>
       <c r="B56" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>27</v>
@@ -5877,10 +5913,10 @@
     <row r="57" spans="1:18">
       <c r="A57" s="2"/>
       <c r="B57" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>27</v>
@@ -5931,10 +5967,10 @@
     <row r="58" spans="1:18">
       <c r="A58" s="2"/>
       <c r="B58" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>27</v>
@@ -5943,103 +5979,67 @@
         <v>0</v>
       </c>
       <c r="F58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="G58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="H58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="I58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="J58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="K58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="L58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="M58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="N58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="O58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="P58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="Q58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
       <c r="R58" s="3">
-        <v>0.9500000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="2"/>
-      <c r="B59" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" s="3">
-        <v>0</v>
-      </c>
-      <c r="F59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="G59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="H59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="I59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="J59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="K59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="L59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="M59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="N59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="O59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="P59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="Q59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
-      <c r="R59" s="3">
-        <v>0.6594636339893744</v>
-      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
     </row>
     <row r="60" spans="1:18">
-      <c r="A60" s="2"/>
+      <c r="A60" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B60" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>26</v>
@@ -6048,52 +6048,52 @@
         <v>27</v>
       </c>
       <c r="E60" s="3">
-        <v>0.3538</v>
+        <v>0</v>
       </c>
       <c r="F60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="G60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="H60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="I60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="J60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="K60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="L60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="M60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="N60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="O60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="P60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
       <c r="R60" s="3">
-        <v>0.9499999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="2"/>
       <c r="B61" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>26</v>
@@ -6102,7 +6102,7 @@
         <v>27</v>
       </c>
       <c r="E61" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F61" s="3">
         <v>0</v>
@@ -6147,7 +6147,7 @@
     <row r="62" spans="1:18">
       <c r="A62" s="2"/>
       <c r="B62" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>26</v>
@@ -6159,49 +6159,49 @@
         <v>0</v>
       </c>
       <c r="F62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="G62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="H62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="J62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="K62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="L62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="M62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="N62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="O62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="P62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="Q62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="R62" s="3">
-        <v>0.3405363660106256</v>
+        <v>0.9500000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="2"/>
       <c r="B63" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>26</v>
@@ -6213,49 +6213,49 @@
         <v>0</v>
       </c>
       <c r="F63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="G63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="H63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="I63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="J63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="K63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="L63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="M63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="N63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="O63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="P63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="Q63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
       <c r="R63" s="3">
-        <v>0</v>
+        <v>0.6340534786265133</v>
       </c>
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="2"/>
       <c r="B64" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>26</v>
@@ -6264,52 +6264,52 @@
         <v>27</v>
       </c>
       <c r="E64" s="3">
-        <v>0.8997000000000001</v>
+        <v>0.3538</v>
       </c>
       <c r="F64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="G64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="H64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="I64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="J64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="K64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="L64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="M64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="N64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="O64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="P64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="Q64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="R64" s="3">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="2"/>
       <c r="B65" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>26</v>
@@ -6318,52 +6318,52 @@
         <v>27</v>
       </c>
       <c r="E65" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="G65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="H65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="I65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="J65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="K65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="L65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="M65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="N65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="O65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="P65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="Q65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="R65" s="3">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="2"/>
       <c r="B66" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>26</v>
@@ -6375,49 +6375,49 @@
         <v>0</v>
       </c>
       <c r="F66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="G66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="H66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="I66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="J66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="K66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="L66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="M66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="N66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="O66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="P66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="Q66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
       <c r="R66" s="3">
-        <v>0</v>
+        <v>0.1302211409356291</v>
       </c>
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="2"/>
       <c r="B67" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>26</v>
@@ -6471,7 +6471,7 @@
     <row r="68" spans="1:18">
       <c r="A68" s="2"/>
       <c r="B68" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>26</v>
@@ -6480,55 +6480,55 @@
         <v>27</v>
       </c>
       <c r="E68" s="3">
-        <v>0</v>
+        <v>0.8997000000000001</v>
       </c>
       <c r="F68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="G68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="H68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="I68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="J68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="K68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="L68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="M68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="N68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="O68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="P68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="Q68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="R68" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="2"/>
       <c r="B69" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>27</v>
@@ -6537,52 +6537,52 @@
         <v>0</v>
       </c>
       <c r="F69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="G69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="H69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="I69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="J69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="K69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="L69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="M69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="N69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="O69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="P69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="Q69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="R69" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="A70" s="2"/>
       <c r="B70" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>27</v>
@@ -6633,10 +6633,10 @@
     <row r="71" spans="1:18">
       <c r="A71" s="2"/>
       <c r="B71" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>27</v>
@@ -6645,52 +6645,52 @@
         <v>0</v>
       </c>
       <c r="F71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="G71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="H71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="I71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="J71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="K71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="L71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="M71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="N71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="O71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="P71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="Q71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
       <c r="R71" s="3">
-        <v>7114536.62875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="2"/>
       <c r="B72" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>27</v>
@@ -6699,112 +6699,112 @@
         <v>0</v>
       </c>
       <c r="F72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="G72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="H72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="I72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="J72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="K72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="L72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="M72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="N72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="O72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="P72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="Q72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
       <c r="R72" s="3">
-        <v>27831157.15001833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:18">
       <c r="A73" s="2"/>
       <c r="B73" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E73" s="3">
-        <v>3317810.965630114</v>
+        <v>0</v>
       </c>
       <c r="F73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="G73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="H73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="I73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="J73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="K73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="L73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="M73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="N73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="O73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="P73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="Q73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
       <c r="R73" s="3">
-        <v>8908763.192053726</v>
+        <v>1.818727301211163e-12</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="2"/>
       <c r="B74" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E74" s="3">
-        <v>4095441.930000001</v>
+        <v>0</v>
       </c>
       <c r="F74" s="3">
         <v>0</v>
@@ -6849,10 +6849,10 @@
     <row r="75" spans="1:18">
       <c r="A75" s="2"/>
       <c r="B75" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>27</v>
@@ -6861,52 +6861,52 @@
         <v>0</v>
       </c>
       <c r="F75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="G75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="H75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="I75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="J75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="K75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="L75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="M75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="N75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="O75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="P75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="Q75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
       <c r="R75" s="3">
-        <v>38488877.9496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="A76" s="2"/>
       <c r="B76" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>27</v>
@@ -6915,166 +6915,166 @@
         <v>0</v>
       </c>
       <c r="F76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="G76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="H76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="I76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="J76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="K76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="L76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="M76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="N76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="O76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="P76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="Q76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
       <c r="R76" s="3">
-        <v>0</v>
+        <v>7114536.62875</v>
       </c>
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="2"/>
       <c r="B77" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E77" s="3">
-        <v>3248848.027554</v>
+        <v>0</v>
       </c>
       <c r="F77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="G77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="H77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="I77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="J77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="K77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="L77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="M77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="N77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="O77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="P77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="Q77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
       <c r="R77" s="3">
-        <v>3430483.079</v>
+        <v>26758779.55304296</v>
       </c>
     </row>
     <row r="78" spans="1:18">
       <c r="A78" s="2"/>
       <c r="B78" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E78" s="3">
-        <v>0</v>
+        <v>3317810.965630114</v>
       </c>
       <c r="F78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="G78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="H78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="I78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="J78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="K78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="L78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="M78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="N78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="O78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="P78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="Q78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
       <c r="R78" s="3">
-        <v>8367031.899999999</v>
+        <v>8908763.192053726</v>
       </c>
     </row>
     <row r="79" spans="1:18">
       <c r="A79" s="2"/>
       <c r="B79" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E79" s="3">
-        <v>0</v>
+        <v>4095441.930000001</v>
       </c>
       <c r="F79" s="3">
         <v>0</v>
@@ -7119,10 +7119,10 @@
     <row r="80" spans="1:18">
       <c r="A80" s="2"/>
       <c r="B80" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>27</v>
@@ -7131,52 +7131,52 @@
         <v>0</v>
       </c>
       <c r="F80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="G80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="H80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="I80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="J80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="K80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="L80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="M80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="N80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="O80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="P80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="Q80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
       <c r="R80" s="3">
-        <v>0</v>
+        <v>5275858.526241147</v>
       </c>
     </row>
     <row r="81" spans="1:18">
       <c r="A81" s="2"/>
       <c r="B81" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>27</v>
@@ -7227,72 +7227,342 @@
     <row r="82" spans="1:18">
       <c r="A82" s="2"/>
       <c r="B82" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="D82" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E82" s="3">
-        <v>0</v>
+        <v>3248848.027554</v>
       </c>
       <c r="F82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="G82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="H82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="I82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="J82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="K82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="L82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="M82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="N82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="O82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="P82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="Q82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
       <c r="R82" s="3">
-        <v>12480159.33241911</v>
+        <v>3430483.079</v>
       </c>
     </row>
     <row r="83" spans="1:18">
       <c r="A83" s="2"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="N83" s="3"/>
+      <c r="B83" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="3">
+        <v>0</v>
+      </c>
+      <c r="F83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="G83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="H83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="I83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="J83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="K83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="L83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="M83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="N83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="O83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="P83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="Q83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+      <c r="R83" s="3">
+        <v>8367031.899999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" s="2"/>
+      <c r="B84" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" s="3">
+        <v>0</v>
+      </c>
+      <c r="F84" s="3">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3">
+        <v>0</v>
+      </c>
+      <c r="H84" s="3">
+        <v>0</v>
+      </c>
+      <c r="I84" s="3">
+        <v>0</v>
+      </c>
+      <c r="J84" s="3">
+        <v>0</v>
+      </c>
+      <c r="K84" s="3">
+        <v>0</v>
+      </c>
+      <c r="L84" s="3">
+        <v>0</v>
+      </c>
+      <c r="M84" s="3">
+        <v>0</v>
+      </c>
+      <c r="N84" s="3">
+        <v>0</v>
+      </c>
+      <c r="O84" s="3">
+        <v>0</v>
+      </c>
+      <c r="P84" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="3">
+        <v>0</v>
+      </c>
+      <c r="R84" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" s="2"/>
+      <c r="B85" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" s="3">
+        <v>0</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
+      <c r="G85" s="3">
+        <v>0</v>
+      </c>
+      <c r="H85" s="3">
+        <v>0</v>
+      </c>
+      <c r="I85" s="3">
+        <v>0</v>
+      </c>
+      <c r="J85" s="3">
+        <v>0</v>
+      </c>
+      <c r="K85" s="3">
+        <v>0</v>
+      </c>
+      <c r="L85" s="3">
+        <v>0</v>
+      </c>
+      <c r="M85" s="3">
+        <v>0</v>
+      </c>
+      <c r="N85" s="3">
+        <v>0</v>
+      </c>
+      <c r="O85" s="3">
+        <v>0</v>
+      </c>
+      <c r="P85" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q85" s="3">
+        <v>0</v>
+      </c>
+      <c r="R85" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="A86" s="2"/>
+      <c r="B86" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E86" s="3">
+        <v>0</v>
+      </c>
+      <c r="F86" s="3">
+        <v>0</v>
+      </c>
+      <c r="G86" s="3">
+        <v>0</v>
+      </c>
+      <c r="H86" s="3">
+        <v>0</v>
+      </c>
+      <c r="I86" s="3">
+        <v>0</v>
+      </c>
+      <c r="J86" s="3">
+        <v>0</v>
+      </c>
+      <c r="K86" s="3">
+        <v>0</v>
+      </c>
+      <c r="L86" s="3">
+        <v>0</v>
+      </c>
+      <c r="M86" s="3">
+        <v>0</v>
+      </c>
+      <c r="N86" s="3">
+        <v>0</v>
+      </c>
+      <c r="O86" s="3">
+        <v>0</v>
+      </c>
+      <c r="P86" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="3">
+        <v>0</v>
+      </c>
+      <c r="R86" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="A87" s="2"/>
+      <c r="B87" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="3">
+        <v>0</v>
+      </c>
+      <c r="F87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="G87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="H87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="I87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="J87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="K87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="L87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="M87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="N87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="O87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="P87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="Q87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+      <c r="R87" s="3">
+        <v>46765556.35275333</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="A88" s="2"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>